<commit_message>
Created proper structure. Updated excel file and test case named are generated in test case section.
</commit_message>
<xml_diff>
--- a/Data/locations.xlsx
+++ b/Data/locations.xlsx
@@ -1,32 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PackageSelection\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B370768-6F41-4A02-92E8-1D26567CD608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -51,48 +31,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
-    <font>
-      <sz val="10"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="6">
+    <font>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FF0C0D0E"/>
       <name val="Inherit"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF0000FF"/>
       <name val="Consolas"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF0000FF"/>
       <name val="Consolas"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Consolas"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,63 +71,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -346,29 +305,24 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="16.88"/>
+    <col customWidth="1" min="2" max="2" width="60.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -379,24 +333,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="str">
-        <f t="shared" ref="A2:A4" si="0">"Run GS for " &amp; MID(B2,FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7)) + 1,FIND(CHAR(160),SUBSTITUTE(B2,".",CHAR(160),3)) - 1 - (FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7))))</f>
-        <v>Run GS for orccf</v>
-      </c>
+    <row r="2">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f t="shared" ref="C2:C4" si="1">MID(B2,FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7)) + 1,FIND(CHAR(160),SUBSTITUTE(B2,".",CHAR(160),3)) - 1 - (FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7))))</f>
+        <f t="shared" ref="C2:C3" si="1">MID(B2,FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7)) + 1,FIND(CHAR(160),SUBSTITUTE(B2,".",CHAR(160),3)) - 1 - (FIND(CHAR(160),SUBSTITUTE(B2,"/",CHAR(160),7))))</f>
         <v>orccf</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Run GS for orcmf</v>
-      </c>
+    <row r="3">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -405,43 +351,41 @@
         <v>orcmf</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13">
       <c r="B13" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Logic to Append the results file if it exists and create new one if not. Used to handle rerun scenario.
</commit_message>
<xml_diff>
--- a/Data/locations.xlsx
+++ b/Data/locations.xlsx
@@ -43,235 +43,235 @@
     <t>${expectedCremationNoFacilities}</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/sacramento/affordable-cremation-funeral-center-north-sacramento/caacn.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/sacramento/affordable-cremation-funeral-center-north-sacramento/caacn.html</t>
   </si>
   <si>
     <t>caacn</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/roseville/affordable-cremation-funeral-service-roseville/caacr.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/roseville/affordable-cremation-funeral-service-roseville/caacr.html</t>
   </si>
   <si>
     <t>caacr</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/sacramento/affordable-cremation-funeral-center-south-sacramento/caacs.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/sacramento/affordable-cremation-funeral-center-south-sacramento/caacs.html</t>
   </si>
   <si>
     <t>caacs</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/placerville/el-dorado-funeral-cremation-services-placerville/caaed.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/placerville/el-dorado-funeral-cremation-services-placerville/caaed.html</t>
   </si>
   <si>
     <t>caaed</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/chico/affordable-mortuary/cabam.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/chico/affordable-mortuary/cabam.html</t>
   </si>
   <si>
     <t>cabam</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/roseville/blue-oaks-cremation-burial-services/cablo.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/roseville/blue-oaks-cremation-burial-services/cablo.html</t>
   </si>
   <si>
     <t>cablo</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/chico/brusie-funeral-home/cabru.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/chico/brusie-funeral-home/cabru.html</t>
   </si>
   <si>
     <t>cabru</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/jackson/daneri-mortuary/cadan.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/jackson/daneri-mortuary/cadan.html</t>
   </si>
   <si>
     <t>cadan</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/pine-grove/amador-hills-cremation-funeral-service/cadll.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/pine-grove/amador-hills-cremation-funeral-service/cadll.html</t>
   </si>
   <si>
     <t>cadll</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/orange/omega-society/caoms.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/orange/omega-society/caoms.html</t>
   </si>
   <si>
     <t>caoms</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/california/yuba-city/ullrey-memorial-chapel/caulm.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/california/yuba-city/ullrey-memorial-chapel/caulm.html</t>
   </si>
   <si>
     <t>caulm</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/denver/a-basic-cremation/coabd.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/denver/a-basic-cremation/coabd.html</t>
   </si>
   <si>
     <t>coabd</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/arvada/aspen-mortuaries-arvada/coama.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/arvada/aspen-mortuaries-arvada/coama.html</t>
   </si>
   <si>
     <t>coama</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/commerce-city/romero-funeral-home-and-cremations-commerce-city/coamc.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/commerce-city/romero-funeral-home-and-cremations-commerce-city/coamc.html</t>
   </si>
   <si>
     <t>coamc</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/lakewood/aspen-mortuaries-lakewood/coaml.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/lakewood/aspen-mortuaries-lakewood/coaml.html</t>
   </si>
   <si>
     <t>coaml</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/colorado-springs/all-states-cremation-colorado-springs/coasc.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/colorado-springs/all-states-cremation-colorado-springs/coasc.html</t>
   </si>
   <si>
     <t>coasc</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/littleton/all-states-cremation-centennial/coasl.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/littleton/all-states-cremation-centennial/coasl.html</t>
   </si>
   <si>
     <t>coasl</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/wheat-ridge/all-states-cremation-wheat-ridge/coasr.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/wheat-ridge/all-states-cremation-wheat-ridge/coasr.html</t>
   </si>
   <si>
     <t>coasr</t>
   </si>
   <si>
-    <t>http://staging.afterall.com/funeral-cremation/colorado/westminster/all-states-cremation-westminster/coasw.html</t>
+    <t>http://staging.altogetherfuneral.com/funeral-cremation/colorado/westminster/all-states-cremation-westminster/coasw.html</t>
   </si>
   <si>
     <t>coasw</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/colorado-springs/all-veterans-funeral-cremation-colorado-springs/coavc.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/colorado-springs/all-veterans-funeral-cremation-colorado-springs/coavc.html</t>
   </si>
   <si>
     <t>coavc</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/littleton/all-veterans-funeral-cremation-centennial/coavl.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/littleton/all-veterans-funeral-cremation-centennial/coavl.html</t>
   </si>
   <si>
     <t>coavl</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/wheat-ridge/all-veterans-funeral-cremation-wheat-ridge/coavr.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/wheat-ridge/all-veterans-funeral-cremation-wheat-ridge/coavr.html</t>
   </si>
   <si>
     <t>coavr</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/westminster/all-veterans-funeral-cremation-westminster/coavw.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/westminster/all-veterans-funeral-cremation-westminster/coavw.html</t>
   </si>
   <si>
     <t>coavw</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/parker/ponderosa-valley-funeral-services/copvp.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/parker/ponderosa-valley-funeral-services/copvp.html</t>
   </si>
   <si>
     <t>copvp</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/aurora/romero-funeral-home-and-cremations-aurora/coroa.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/aurora/romero-funeral-home-and-cremations-aurora/coroa.html</t>
   </si>
   <si>
     <t>coroa</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/denver/romero-funeral-home-and-cremations-denver/corod.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/denver/romero-funeral-home-and-cremations-denver/corod.html</t>
   </si>
   <si>
     <t>corod</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/lakewood/romero-funeral-home-and-cremations-lakewood/corol.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/lakewood/romero-funeral-home-and-cremations-lakewood/corol.html</t>
   </si>
   <si>
     <t>corol</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/colorado-springs/the-springs-funeral-services-platte/cotsf.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/colorado-springs/the-springs-funeral-services-platte/cotsf.html</t>
   </si>
   <si>
     <t>cotsf</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/colorado/colorado-springs/the-springs-funeral-services-north/cotsn.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/colorado/colorado-springs/the-springs-funeral-services-north/cotsn.html</t>
   </si>
   <si>
     <t>cotsn</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/canby/canby-funeral-chapel/orccf.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/canby/canby-funeral-chapel/orccf.html</t>
   </si>
   <si>
     <t>orccf</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/molalla/molalla-funeral-chapel/orcmf.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/molalla/molalla-funeral-chapel/orcmf.html</t>
   </si>
   <si>
     <t>orcmf</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/portland/crown-cremation-services-portland/orcmp.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/portland/crown-cremation-services-portland/orcmp.html</t>
   </si>
   <si>
     <t>orcmp</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/salem/crown-cremation-services-salem/orcms.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/salem/crown-cremation-services-salem/orcms.html</t>
   </si>
   <si>
     <t>orcms</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/tualatin/crown-cremation-services-tualatin/orcmt.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/tualatin/crown-cremation-services-tualatin/orcmt.html</t>
   </si>
   <si>
     <t>orcmt</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/eugene/alpha-cremation-services/ormac.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/eugene/alpha-cremation-services/ormac.html</t>
   </si>
   <si>
     <t>ormac</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/eugene/lane-memorial-funeral-home/ormlm.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/eugene/lane-memorial-funeral-home/ormlm.html</t>
   </si>
   <si>
     <t>ormlm</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/junction-city/murphy-musgrove-funeral-home/ormmm.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/junction-city/murphy-musgrove-funeral-home/ormmm.html</t>
   </si>
   <si>
     <t>ormmm</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/springfield/springfield-memorial-funeral-home/ormsm.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/springfield/springfield-memorial-funeral-home/ormsm.html</t>
   </si>
   <si>
     <t>ormsm</t>
   </si>
   <si>
-    <t>https://staging.afterall.com/funeral-cremation/oregon/eugene/musgrove-family-mortuary/ormwl.html</t>
+    <t>https://staging.altogetherfuneral.com/funeral-cremation/oregon/eugene/musgrove-family-mortuary/ormwl.html</t>
   </si>
   <si>
     <t>ormwl</t>
@@ -299,6 +299,9 @@
     </font>
     <font>
       <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -306,9 +309,6 @@
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -354,6 +354,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -695,7 +698,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for caacs</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -728,7 +731,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for caaed</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -761,7 +764,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for cabam</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -794,7 +797,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for cablo</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -827,7 +830,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for cabru</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -860,7 +863,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for cadan</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -893,7 +896,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for cadll</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -926,7 +929,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for caoms</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -959,7 +962,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for caulm</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -992,7 +995,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for coabd</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1028,7 +1031,7 @@
       <c r="B14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="7">
@@ -1061,7 +1064,7 @@
       <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="7">
@@ -1094,7 +1097,7 @@
       <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="7">
@@ -1127,7 +1130,7 @@
       <c r="B17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="7">
@@ -1148,7 +1151,7 @@
       <c r="I17" s="7">
         <v>4.0</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="12">
         <v>3.0</v>
       </c>
     </row>
@@ -1157,10 +1160,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for coasl</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="7">
@@ -1193,7 +1196,7 @@
       <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="7">
@@ -1223,10 +1226,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for coasw</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="7">
@@ -1259,7 +1262,7 @@
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="7">
@@ -1292,7 +1295,7 @@
       <c r="B22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="7">
@@ -1325,7 +1328,7 @@
       <c r="B23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="7">
@@ -1355,10 +1358,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for coavw</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="7">
@@ -1391,7 +1394,7 @@
       <c r="B25" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="7">
@@ -1421,10 +1424,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for coroa</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="7">
@@ -1454,10 +1457,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for corod</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="7">
@@ -1490,7 +1493,7 @@
       <c r="B28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="7">
@@ -1520,10 +1523,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for cotsf</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="7">
@@ -1553,10 +1556,10 @@
         <f t="shared" si="1"/>
         <v>Run GS for cotsn</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="7">
@@ -1685,7 +1688,7 @@
         <f t="shared" si="1"/>
         <v>Run GS for orcms</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="9" t="s">
         <v>74</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -1912,2955 +1915,2945 @@
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="14"/>
+      <c r="B41" s="15"/>
     </row>
     <row r="42">
-      <c r="B42" s="14"/>
+      <c r="B42" s="15"/>
     </row>
     <row r="43">
-      <c r="B43" s="14"/>
+      <c r="B43" s="15"/>
     </row>
     <row r="44">
-      <c r="B44" s="14"/>
+      <c r="B44" s="15"/>
     </row>
     <row r="45">
-      <c r="B45" s="14"/>
+      <c r="B45" s="15"/>
     </row>
     <row r="46">
-      <c r="B46" s="14"/>
+      <c r="B46" s="15"/>
     </row>
     <row r="47">
-      <c r="B47" s="14"/>
+      <c r="B47" s="15"/>
     </row>
     <row r="48">
-      <c r="B48" s="14"/>
+      <c r="B48" s="15"/>
     </row>
     <row r="49">
-      <c r="B49" s="14"/>
+      <c r="B49" s="15"/>
     </row>
     <row r="50">
-      <c r="B50" s="14"/>
+      <c r="B50" s="15"/>
     </row>
     <row r="51">
-      <c r="B51" s="14"/>
+      <c r="B51" s="15"/>
     </row>
     <row r="52">
-      <c r="B52" s="14"/>
+      <c r="B52" s="15"/>
     </row>
     <row r="53">
-      <c r="B53" s="14"/>
+      <c r="B53" s="15"/>
     </row>
     <row r="54">
-      <c r="B54" s="14"/>
+      <c r="B54" s="15"/>
     </row>
     <row r="55">
-      <c r="B55" s="14"/>
+      <c r="B55" s="15"/>
     </row>
     <row r="56">
-      <c r="B56" s="14"/>
+      <c r="B56" s="15"/>
     </row>
     <row r="57">
-      <c r="B57" s="14"/>
+      <c r="B57" s="15"/>
     </row>
     <row r="58">
-      <c r="B58" s="14"/>
+      <c r="B58" s="15"/>
     </row>
     <row r="59">
-      <c r="B59" s="14"/>
+      <c r="B59" s="15"/>
     </row>
     <row r="60">
-      <c r="B60" s="14"/>
+      <c r="B60" s="15"/>
     </row>
     <row r="61">
-      <c r="B61" s="14"/>
+      <c r="B61" s="15"/>
     </row>
     <row r="62">
-      <c r="B62" s="14"/>
+      <c r="B62" s="15"/>
     </row>
     <row r="63">
-      <c r="B63" s="14"/>
+      <c r="B63" s="15"/>
     </row>
     <row r="64">
-      <c r="B64" s="14"/>
+      <c r="B64" s="15"/>
     </row>
     <row r="65">
-      <c r="B65" s="14"/>
+      <c r="B65" s="15"/>
     </row>
     <row r="66">
-      <c r="B66" s="14"/>
+      <c r="B66" s="15"/>
     </row>
     <row r="67">
-      <c r="B67" s="14"/>
+      <c r="B67" s="15"/>
     </row>
     <row r="68">
-      <c r="B68" s="14"/>
+      <c r="B68" s="15"/>
     </row>
     <row r="69">
-      <c r="B69" s="14"/>
+      <c r="B69" s="15"/>
     </row>
     <row r="70">
-      <c r="B70" s="14"/>
+      <c r="B70" s="15"/>
     </row>
     <row r="71">
-      <c r="B71" s="14"/>
+      <c r="B71" s="15"/>
     </row>
     <row r="72">
-      <c r="B72" s="14"/>
+      <c r="B72" s="15"/>
     </row>
     <row r="73">
-      <c r="B73" s="14"/>
+      <c r="B73" s="15"/>
     </row>
     <row r="74">
-      <c r="B74" s="14"/>
+      <c r="B74" s="15"/>
     </row>
     <row r="75">
-      <c r="B75" s="14"/>
+      <c r="B75" s="15"/>
     </row>
     <row r="76">
-      <c r="B76" s="14"/>
+      <c r="B76" s="15"/>
     </row>
     <row r="77">
-      <c r="B77" s="14"/>
+      <c r="B77" s="15"/>
     </row>
     <row r="78">
-      <c r="B78" s="14"/>
+      <c r="B78" s="15"/>
     </row>
     <row r="79">
-      <c r="B79" s="14"/>
+      <c r="B79" s="15"/>
     </row>
     <row r="80">
-      <c r="B80" s="14"/>
+      <c r="B80" s="15"/>
     </row>
     <row r="81">
-      <c r="B81" s="14"/>
+      <c r="B81" s="15"/>
     </row>
     <row r="82">
-      <c r="B82" s="14"/>
+      <c r="B82" s="15"/>
     </row>
     <row r="83">
-      <c r="B83" s="14"/>
+      <c r="B83" s="15"/>
     </row>
     <row r="84">
-      <c r="B84" s="14"/>
+      <c r="B84" s="15"/>
     </row>
     <row r="85">
-      <c r="B85" s="14"/>
+      <c r="B85" s="15"/>
     </row>
     <row r="86">
-      <c r="B86" s="14"/>
+      <c r="B86" s="15"/>
     </row>
     <row r="87">
-      <c r="B87" s="14"/>
+      <c r="B87" s="15"/>
     </row>
     <row r="88">
-      <c r="B88" s="14"/>
+      <c r="B88" s="15"/>
     </row>
     <row r="89">
-      <c r="B89" s="14"/>
+      <c r="B89" s="15"/>
     </row>
     <row r="90">
-      <c r="B90" s="14"/>
+      <c r="B90" s="15"/>
     </row>
     <row r="91">
-      <c r="B91" s="14"/>
+      <c r="B91" s="15"/>
     </row>
     <row r="92">
-      <c r="B92" s="14"/>
+      <c r="B92" s="15"/>
     </row>
     <row r="93">
-      <c r="B93" s="14"/>
+      <c r="B93" s="15"/>
     </row>
     <row r="94">
-      <c r="B94" s="14"/>
+      <c r="B94" s="15"/>
     </row>
     <row r="95">
-      <c r="B95" s="14"/>
+      <c r="B95" s="15"/>
     </row>
     <row r="96">
-      <c r="B96" s="14"/>
+      <c r="B96" s="15"/>
     </row>
     <row r="97">
-      <c r="B97" s="14"/>
+      <c r="B97" s="15"/>
     </row>
     <row r="98">
-      <c r="B98" s="14"/>
+      <c r="B98" s="15"/>
     </row>
     <row r="99">
-      <c r="B99" s="14"/>
+      <c r="B99" s="15"/>
     </row>
     <row r="100">
-      <c r="B100" s="14"/>
+      <c r="B100" s="15"/>
     </row>
     <row r="101">
-      <c r="B101" s="14"/>
+      <c r="B101" s="15"/>
     </row>
     <row r="102">
-      <c r="B102" s="14"/>
+      <c r="B102" s="15"/>
     </row>
     <row r="103">
-      <c r="B103" s="14"/>
+      <c r="B103" s="15"/>
     </row>
     <row r="104">
-      <c r="B104" s="14"/>
+      <c r="B104" s="15"/>
     </row>
     <row r="105">
-      <c r="B105" s="14"/>
+      <c r="B105" s="15"/>
     </row>
     <row r="106">
-      <c r="B106" s="14"/>
+      <c r="B106" s="15"/>
     </row>
     <row r="107">
-      <c r="B107" s="14"/>
+      <c r="B107" s="15"/>
     </row>
     <row r="108">
-      <c r="B108" s="14"/>
+      <c r="B108" s="15"/>
     </row>
     <row r="109">
-      <c r="B109" s="14"/>
+      <c r="B109" s="15"/>
     </row>
     <row r="110">
-      <c r="B110" s="14"/>
+      <c r="B110" s="15"/>
     </row>
     <row r="111">
-      <c r="B111" s="14"/>
+      <c r="B111" s="15"/>
     </row>
     <row r="112">
-      <c r="B112" s="14"/>
+      <c r="B112" s="15"/>
     </row>
     <row r="113">
-      <c r="B113" s="14"/>
+      <c r="B113" s="15"/>
     </row>
     <row r="114">
-      <c r="B114" s="14"/>
+      <c r="B114" s="15"/>
     </row>
     <row r="115">
-      <c r="B115" s="14"/>
+      <c r="B115" s="15"/>
     </row>
     <row r="116">
-      <c r="B116" s="14"/>
+      <c r="B116" s="15"/>
     </row>
     <row r="117">
-      <c r="B117" s="14"/>
+      <c r="B117" s="15"/>
     </row>
     <row r="118">
-      <c r="B118" s="14"/>
+      <c r="B118" s="15"/>
     </row>
     <row r="119">
-      <c r="B119" s="14"/>
+      <c r="B119" s="15"/>
     </row>
     <row r="120">
-      <c r="B120" s="14"/>
+      <c r="B120" s="15"/>
     </row>
     <row r="121">
-      <c r="B121" s="14"/>
+      <c r="B121" s="15"/>
     </row>
     <row r="122">
-      <c r="B122" s="14"/>
+      <c r="B122" s="15"/>
     </row>
     <row r="123">
-      <c r="B123" s="14"/>
+      <c r="B123" s="15"/>
     </row>
     <row r="124">
-      <c r="B124" s="14"/>
+      <c r="B124" s="15"/>
     </row>
     <row r="125">
-      <c r="B125" s="14"/>
+      <c r="B125" s="15"/>
     </row>
     <row r="126">
-      <c r="B126" s="14"/>
+      <c r="B126" s="15"/>
     </row>
     <row r="127">
-      <c r="B127" s="14"/>
+      <c r="B127" s="15"/>
     </row>
     <row r="128">
-      <c r="B128" s="14"/>
+      <c r="B128" s="15"/>
     </row>
     <row r="129">
-      <c r="B129" s="14"/>
+      <c r="B129" s="15"/>
     </row>
     <row r="130">
-      <c r="B130" s="14"/>
+      <c r="B130" s="15"/>
     </row>
     <row r="131">
-      <c r="B131" s="14"/>
+      <c r="B131" s="15"/>
     </row>
     <row r="132">
-      <c r="B132" s="14"/>
+      <c r="B132" s="15"/>
     </row>
     <row r="133">
-      <c r="B133" s="14"/>
+      <c r="B133" s="15"/>
     </row>
     <row r="134">
-      <c r="B134" s="14"/>
+      <c r="B134" s="15"/>
     </row>
     <row r="135">
-      <c r="B135" s="14"/>
+      <c r="B135" s="15"/>
     </row>
     <row r="136">
-      <c r="B136" s="14"/>
+      <c r="B136" s="15"/>
     </row>
     <row r="137">
-      <c r="B137" s="14"/>
+      <c r="B137" s="15"/>
     </row>
     <row r="138">
-      <c r="B138" s="14"/>
+      <c r="B138" s="15"/>
     </row>
     <row r="139">
-      <c r="B139" s="14"/>
+      <c r="B139" s="15"/>
     </row>
     <row r="140">
-      <c r="B140" s="14"/>
+      <c r="B140" s="15"/>
     </row>
     <row r="141">
-      <c r="B141" s="14"/>
+      <c r="B141" s="15"/>
     </row>
     <row r="142">
-      <c r="B142" s="14"/>
+      <c r="B142" s="15"/>
     </row>
     <row r="143">
-      <c r="B143" s="14"/>
+      <c r="B143" s="15"/>
     </row>
     <row r="144">
-      <c r="B144" s="14"/>
+      <c r="B144" s="15"/>
     </row>
     <row r="145">
-      <c r="B145" s="14"/>
+      <c r="B145" s="15"/>
     </row>
     <row r="146">
-      <c r="B146" s="14"/>
+      <c r="B146" s="15"/>
     </row>
     <row r="147">
-      <c r="B147" s="14"/>
+      <c r="B147" s="15"/>
     </row>
     <row r="148">
-      <c r="B148" s="14"/>
+      <c r="B148" s="15"/>
     </row>
     <row r="149">
-      <c r="B149" s="14"/>
+      <c r="B149" s="15"/>
     </row>
     <row r="150">
-      <c r="B150" s="14"/>
+      <c r="B150" s="15"/>
     </row>
     <row r="151">
-      <c r="B151" s="14"/>
+      <c r="B151" s="15"/>
     </row>
     <row r="152">
-      <c r="B152" s="14"/>
+      <c r="B152" s="15"/>
     </row>
     <row r="153">
-      <c r="B153" s="14"/>
+      <c r="B153" s="15"/>
     </row>
     <row r="154">
-      <c r="B154" s="14"/>
+      <c r="B154" s="15"/>
     </row>
     <row r="155">
-      <c r="B155" s="14"/>
+      <c r="B155" s="15"/>
     </row>
     <row r="156">
-      <c r="B156" s="14"/>
+      <c r="B156" s="15"/>
     </row>
     <row r="157">
-      <c r="B157" s="14"/>
+      <c r="B157" s="15"/>
     </row>
     <row r="158">
-      <c r="B158" s="14"/>
+      <c r="B158" s="15"/>
     </row>
     <row r="159">
-      <c r="B159" s="14"/>
+      <c r="B159" s="15"/>
     </row>
     <row r="160">
-      <c r="B160" s="14"/>
+      <c r="B160" s="15"/>
     </row>
     <row r="161">
-      <c r="B161" s="14"/>
+      <c r="B161" s="15"/>
     </row>
     <row r="162">
-      <c r="B162" s="14"/>
+      <c r="B162" s="15"/>
     </row>
     <row r="163">
-      <c r="B163" s="14"/>
+      <c r="B163" s="15"/>
     </row>
     <row r="164">
-      <c r="B164" s="14"/>
+      <c r="B164" s="15"/>
     </row>
     <row r="165">
-      <c r="B165" s="14"/>
+      <c r="B165" s="15"/>
     </row>
     <row r="166">
-      <c r="B166" s="14"/>
+      <c r="B166" s="15"/>
     </row>
     <row r="167">
-      <c r="B167" s="14"/>
+      <c r="B167" s="15"/>
     </row>
     <row r="168">
-      <c r="B168" s="14"/>
+      <c r="B168" s="15"/>
     </row>
     <row r="169">
-      <c r="B169" s="14"/>
+      <c r="B169" s="15"/>
     </row>
     <row r="170">
-      <c r="B170" s="14"/>
+      <c r="B170" s="15"/>
     </row>
     <row r="171">
-      <c r="B171" s="14"/>
+      <c r="B171" s="15"/>
     </row>
     <row r="172">
-      <c r="B172" s="14"/>
+      <c r="B172" s="15"/>
     </row>
     <row r="173">
-      <c r="B173" s="14"/>
+      <c r="B173" s="15"/>
     </row>
     <row r="174">
-      <c r="B174" s="14"/>
+      <c r="B174" s="15"/>
     </row>
     <row r="175">
-      <c r="B175" s="14"/>
+      <c r="B175" s="15"/>
     </row>
     <row r="176">
-      <c r="B176" s="14"/>
+      <c r="B176" s="15"/>
     </row>
     <row r="177">
-      <c r="B177" s="14"/>
+      <c r="B177" s="15"/>
     </row>
     <row r="178">
-      <c r="B178" s="14"/>
+      <c r="B178" s="15"/>
     </row>
     <row r="179">
-      <c r="B179" s="14"/>
+      <c r="B179" s="15"/>
     </row>
     <row r="180">
-      <c r="B180" s="14"/>
+      <c r="B180" s="15"/>
     </row>
     <row r="181">
-      <c r="B181" s="14"/>
+      <c r="B181" s="15"/>
     </row>
     <row r="182">
-      <c r="B182" s="14"/>
+      <c r="B182" s="15"/>
     </row>
     <row r="183">
-      <c r="B183" s="14"/>
+      <c r="B183" s="15"/>
     </row>
     <row r="184">
-      <c r="B184" s="14"/>
+      <c r="B184" s="15"/>
     </row>
     <row r="185">
-      <c r="B185" s="14"/>
+      <c r="B185" s="15"/>
     </row>
     <row r="186">
-      <c r="B186" s="14"/>
+      <c r="B186" s="15"/>
     </row>
     <row r="187">
-      <c r="B187" s="14"/>
+      <c r="B187" s="15"/>
     </row>
     <row r="188">
-      <c r="B188" s="14"/>
+      <c r="B188" s="15"/>
     </row>
     <row r="189">
-      <c r="B189" s="14"/>
+      <c r="B189" s="15"/>
     </row>
     <row r="190">
-      <c r="B190" s="14"/>
+      <c r="B190" s="15"/>
     </row>
     <row r="191">
-      <c r="B191" s="14"/>
+      <c r="B191" s="15"/>
     </row>
     <row r="192">
-      <c r="B192" s="14"/>
+      <c r="B192" s="15"/>
     </row>
     <row r="193">
-      <c r="B193" s="14"/>
+      <c r="B193" s="15"/>
     </row>
     <row r="194">
-      <c r="B194" s="14"/>
+      <c r="B194" s="15"/>
     </row>
     <row r="195">
-      <c r="B195" s="14"/>
+      <c r="B195" s="15"/>
     </row>
     <row r="196">
-      <c r="B196" s="14"/>
+      <c r="B196" s="15"/>
     </row>
     <row r="197">
-      <c r="B197" s="14"/>
+      <c r="B197" s="15"/>
     </row>
     <row r="198">
-      <c r="B198" s="14"/>
+      <c r="B198" s="15"/>
     </row>
     <row r="199">
-      <c r="B199" s="14"/>
+      <c r="B199" s="15"/>
     </row>
     <row r="200">
-      <c r="B200" s="14"/>
+      <c r="B200" s="15"/>
     </row>
     <row r="201">
-      <c r="B201" s="14"/>
+      <c r="B201" s="15"/>
     </row>
     <row r="202">
-      <c r="B202" s="14"/>
+      <c r="B202" s="15"/>
     </row>
     <row r="203">
-      <c r="B203" s="14"/>
+      <c r="B203" s="15"/>
     </row>
     <row r="204">
-      <c r="B204" s="14"/>
+      <c r="B204" s="15"/>
     </row>
     <row r="205">
-      <c r="B205" s="14"/>
+      <c r="B205" s="15"/>
     </row>
     <row r="206">
-      <c r="B206" s="14"/>
+      <c r="B206" s="15"/>
     </row>
     <row r="207">
-      <c r="B207" s="14"/>
+      <c r="B207" s="15"/>
     </row>
     <row r="208">
-      <c r="B208" s="14"/>
+      <c r="B208" s="15"/>
     </row>
     <row r="209">
-      <c r="B209" s="14"/>
+      <c r="B209" s="15"/>
     </row>
     <row r="210">
-      <c r="B210" s="14"/>
+      <c r="B210" s="15"/>
     </row>
     <row r="211">
-      <c r="B211" s="14"/>
+      <c r="B211" s="15"/>
     </row>
     <row r="212">
-      <c r="B212" s="14"/>
+      <c r="B212" s="15"/>
     </row>
     <row r="213">
-      <c r="B213" s="14"/>
+      <c r="B213" s="15"/>
     </row>
     <row r="214">
-      <c r="B214" s="14"/>
+      <c r="B214" s="15"/>
     </row>
     <row r="215">
-      <c r="B215" s="14"/>
+      <c r="B215" s="15"/>
     </row>
     <row r="216">
-      <c r="B216" s="14"/>
+      <c r="B216" s="15"/>
     </row>
     <row r="217">
-      <c r="B217" s="14"/>
+      <c r="B217" s="15"/>
     </row>
     <row r="218">
-      <c r="B218" s="14"/>
+      <c r="B218" s="15"/>
     </row>
     <row r="219">
-      <c r="B219" s="14"/>
+      <c r="B219" s="15"/>
     </row>
     <row r="220">
-      <c r="B220" s="14"/>
+      <c r="B220" s="15"/>
     </row>
     <row r="221">
-      <c r="B221" s="14"/>
+      <c r="B221" s="15"/>
     </row>
     <row r="222">
-      <c r="B222" s="14"/>
+      <c r="B222" s="15"/>
     </row>
     <row r="223">
-      <c r="B223" s="14"/>
+      <c r="B223" s="15"/>
     </row>
     <row r="224">
-      <c r="B224" s="14"/>
+      <c r="B224" s="15"/>
     </row>
     <row r="225">
-      <c r="B225" s="14"/>
+      <c r="B225" s="15"/>
     </row>
     <row r="226">
-      <c r="B226" s="14"/>
+      <c r="B226" s="15"/>
     </row>
     <row r="227">
-      <c r="B227" s="14"/>
+      <c r="B227" s="15"/>
     </row>
     <row r="228">
-      <c r="B228" s="14"/>
+      <c r="B228" s="15"/>
     </row>
     <row r="229">
-      <c r="B229" s="14"/>
+      <c r="B229" s="15"/>
     </row>
     <row r="230">
-      <c r="B230" s="14"/>
+      <c r="B230" s="15"/>
     </row>
     <row r="231">
-      <c r="B231" s="14"/>
+      <c r="B231" s="15"/>
     </row>
     <row r="232">
-      <c r="B232" s="14"/>
+      <c r="B232" s="15"/>
     </row>
     <row r="233">
-      <c r="B233" s="14"/>
+      <c r="B233" s="15"/>
     </row>
     <row r="234">
-      <c r="B234" s="14"/>
+      <c r="B234" s="15"/>
     </row>
     <row r="235">
-      <c r="B235" s="14"/>
+      <c r="B235" s="15"/>
     </row>
     <row r="236">
-      <c r="B236" s="14"/>
+      <c r="B236" s="15"/>
     </row>
     <row r="237">
-      <c r="B237" s="14"/>
+      <c r="B237" s="15"/>
     </row>
     <row r="238">
-      <c r="B238" s="14"/>
+      <c r="B238" s="15"/>
     </row>
     <row r="239">
-      <c r="B239" s="14"/>
+      <c r="B239" s="15"/>
     </row>
     <row r="240">
-      <c r="B240" s="14"/>
+      <c r="B240" s="15"/>
     </row>
     <row r="241">
-      <c r="B241" s="14"/>
+      <c r="B241" s="15"/>
     </row>
     <row r="242">
-      <c r="B242" s="14"/>
+      <c r="B242" s="15"/>
     </row>
     <row r="243">
-      <c r="B243" s="14"/>
+      <c r="B243" s="15"/>
     </row>
     <row r="244">
-      <c r="B244" s="14"/>
+      <c r="B244" s="15"/>
     </row>
     <row r="245">
-      <c r="B245" s="14"/>
+      <c r="B245" s="15"/>
     </row>
     <row r="246">
-      <c r="B246" s="14"/>
+      <c r="B246" s="15"/>
     </row>
     <row r="247">
-      <c r="B247" s="14"/>
+      <c r="B247" s="15"/>
     </row>
     <row r="248">
-      <c r="B248" s="14"/>
+      <c r="B248" s="15"/>
     </row>
     <row r="249">
-      <c r="B249" s="14"/>
+      <c r="B249" s="15"/>
     </row>
     <row r="250">
-      <c r="B250" s="14"/>
+      <c r="B250" s="15"/>
     </row>
     <row r="251">
-      <c r="B251" s="14"/>
+      <c r="B251" s="15"/>
     </row>
     <row r="252">
-      <c r="B252" s="14"/>
+      <c r="B252" s="15"/>
     </row>
     <row r="253">
-      <c r="B253" s="14"/>
+      <c r="B253" s="15"/>
     </row>
     <row r="254">
-      <c r="B254" s="14"/>
+      <c r="B254" s="15"/>
     </row>
     <row r="255">
-      <c r="B255" s="14"/>
+      <c r="B255" s="15"/>
     </row>
     <row r="256">
-      <c r="B256" s="14"/>
+      <c r="B256" s="15"/>
     </row>
     <row r="257">
-      <c r="B257" s="14"/>
+      <c r="B257" s="15"/>
     </row>
     <row r="258">
-      <c r="B258" s="14"/>
+      <c r="B258" s="15"/>
     </row>
     <row r="259">
-      <c r="B259" s="14"/>
+      <c r="B259" s="15"/>
     </row>
     <row r="260">
-      <c r="B260" s="14"/>
+      <c r="B260" s="15"/>
     </row>
     <row r="261">
-      <c r="B261" s="14"/>
+      <c r="B261" s="15"/>
     </row>
     <row r="262">
-      <c r="B262" s="14"/>
+      <c r="B262" s="15"/>
     </row>
     <row r="263">
-      <c r="B263" s="14"/>
+      <c r="B263" s="15"/>
     </row>
     <row r="264">
-      <c r="B264" s="14"/>
+      <c r="B264" s="15"/>
     </row>
     <row r="265">
-      <c r="B265" s="14"/>
+      <c r="B265" s="15"/>
     </row>
     <row r="266">
-      <c r="B266" s="14"/>
+      <c r="B266" s="15"/>
     </row>
     <row r="267">
-      <c r="B267" s="14"/>
+      <c r="B267" s="15"/>
     </row>
     <row r="268">
-      <c r="B268" s="14"/>
+      <c r="B268" s="15"/>
     </row>
     <row r="269">
-      <c r="B269" s="14"/>
+      <c r="B269" s="15"/>
     </row>
     <row r="270">
-      <c r="B270" s="14"/>
+      <c r="B270" s="15"/>
     </row>
     <row r="271">
-      <c r="B271" s="14"/>
+      <c r="B271" s="15"/>
     </row>
     <row r="272">
-      <c r="B272" s="14"/>
+      <c r="B272" s="15"/>
     </row>
     <row r="273">
-      <c r="B273" s="14"/>
+      <c r="B273" s="15"/>
     </row>
     <row r="274">
-      <c r="B274" s="14"/>
+      <c r="B274" s="15"/>
     </row>
     <row r="275">
-      <c r="B275" s="14"/>
+      <c r="B275" s="15"/>
     </row>
     <row r="276">
-      <c r="B276" s="14"/>
+      <c r="B276" s="15"/>
     </row>
     <row r="277">
-      <c r="B277" s="14"/>
+      <c r="B277" s="15"/>
     </row>
     <row r="278">
-      <c r="B278" s="14"/>
+      <c r="B278" s="15"/>
     </row>
     <row r="279">
-      <c r="B279" s="14"/>
+      <c r="B279" s="15"/>
     </row>
     <row r="280">
-      <c r="B280" s="14"/>
+      <c r="B280" s="15"/>
     </row>
     <row r="281">
-      <c r="B281" s="14"/>
+      <c r="B281" s="15"/>
     </row>
     <row r="282">
-      <c r="B282" s="14"/>
+      <c r="B282" s="15"/>
     </row>
     <row r="283">
-      <c r="B283" s="14"/>
+      <c r="B283" s="15"/>
     </row>
     <row r="284">
-      <c r="B284" s="14"/>
+      <c r="B284" s="15"/>
     </row>
     <row r="285">
-      <c r="B285" s="14"/>
+      <c r="B285" s="15"/>
     </row>
     <row r="286">
-      <c r="B286" s="14"/>
+      <c r="B286" s="15"/>
     </row>
     <row r="287">
-      <c r="B287" s="14"/>
+      <c r="B287" s="15"/>
     </row>
     <row r="288">
-      <c r="B288" s="14"/>
+      <c r="B288" s="15"/>
     </row>
     <row r="289">
-      <c r="B289" s="14"/>
+      <c r="B289" s="15"/>
     </row>
     <row r="290">
-      <c r="B290" s="14"/>
+      <c r="B290" s="15"/>
     </row>
     <row r="291">
-      <c r="B291" s="14"/>
+      <c r="B291" s="15"/>
     </row>
     <row r="292">
-      <c r="B292" s="14"/>
+      <c r="B292" s="15"/>
     </row>
     <row r="293">
-      <c r="B293" s="14"/>
+      <c r="B293" s="15"/>
     </row>
     <row r="294">
-      <c r="B294" s="14"/>
+      <c r="B294" s="15"/>
     </row>
     <row r="295">
-      <c r="B295" s="14"/>
+      <c r="B295" s="15"/>
     </row>
     <row r="296">
-      <c r="B296" s="14"/>
+      <c r="B296" s="15"/>
     </row>
     <row r="297">
-      <c r="B297" s="14"/>
+      <c r="B297" s="15"/>
     </row>
     <row r="298">
-      <c r="B298" s="14"/>
+      <c r="B298" s="15"/>
     </row>
     <row r="299">
-      <c r="B299" s="14"/>
+      <c r="B299" s="15"/>
     </row>
     <row r="300">
-      <c r="B300" s="14"/>
+      <c r="B300" s="15"/>
     </row>
     <row r="301">
-      <c r="B301" s="14"/>
+      <c r="B301" s="15"/>
     </row>
     <row r="302">
-      <c r="B302" s="14"/>
+      <c r="B302" s="15"/>
     </row>
     <row r="303">
-      <c r="B303" s="14"/>
+      <c r="B303" s="15"/>
     </row>
     <row r="304">
-      <c r="B304" s="14"/>
+      <c r="B304" s="15"/>
     </row>
     <row r="305">
-      <c r="B305" s="14"/>
+      <c r="B305" s="15"/>
     </row>
     <row r="306">
-      <c r="B306" s="14"/>
+      <c r="B306" s="15"/>
     </row>
     <row r="307">
-      <c r="B307" s="14"/>
+      <c r="B307" s="15"/>
     </row>
     <row r="308">
-      <c r="B308" s="14"/>
+      <c r="B308" s="15"/>
     </row>
     <row r="309">
-      <c r="B309" s="14"/>
+      <c r="B309" s="15"/>
     </row>
     <row r="310">
-      <c r="B310" s="14"/>
+      <c r="B310" s="15"/>
     </row>
     <row r="311">
-      <c r="B311" s="14"/>
+      <c r="B311" s="15"/>
     </row>
     <row r="312">
-      <c r="B312" s="14"/>
+      <c r="B312" s="15"/>
     </row>
     <row r="313">
-      <c r="B313" s="14"/>
+      <c r="B313" s="15"/>
     </row>
     <row r="314">
-      <c r="B314" s="14"/>
+      <c r="B314" s="15"/>
     </row>
     <row r="315">
-      <c r="B315" s="14"/>
+      <c r="B315" s="15"/>
     </row>
     <row r="316">
-      <c r="B316" s="14"/>
+      <c r="B316" s="15"/>
     </row>
     <row r="317">
-      <c r="B317" s="14"/>
+      <c r="B317" s="15"/>
     </row>
     <row r="318">
-      <c r="B318" s="14"/>
+      <c r="B318" s="15"/>
     </row>
     <row r="319">
-      <c r="B319" s="14"/>
+      <c r="B319" s="15"/>
     </row>
     <row r="320">
-      <c r="B320" s="14"/>
+      <c r="B320" s="15"/>
     </row>
     <row r="321">
-      <c r="B321" s="14"/>
+      <c r="B321" s="15"/>
     </row>
     <row r="322">
-      <c r="B322" s="14"/>
+      <c r="B322" s="15"/>
     </row>
     <row r="323">
-      <c r="B323" s="14"/>
+      <c r="B323" s="15"/>
     </row>
     <row r="324">
-      <c r="B324" s="14"/>
+      <c r="B324" s="15"/>
     </row>
     <row r="325">
-      <c r="B325" s="14"/>
+      <c r="B325" s="15"/>
     </row>
     <row r="326">
-      <c r="B326" s="14"/>
+      <c r="B326" s="15"/>
     </row>
     <row r="327">
-      <c r="B327" s="14"/>
+      <c r="B327" s="15"/>
     </row>
     <row r="328">
-      <c r="B328" s="14"/>
+      <c r="B328" s="15"/>
     </row>
     <row r="329">
-      <c r="B329" s="14"/>
+      <c r="B329" s="15"/>
     </row>
     <row r="330">
-      <c r="B330" s="14"/>
+      <c r="B330" s="15"/>
     </row>
     <row r="331">
-      <c r="B331" s="14"/>
+      <c r="B331" s="15"/>
     </row>
     <row r="332">
-      <c r="B332" s="14"/>
+      <c r="B332" s="15"/>
     </row>
     <row r="333">
-      <c r="B333" s="14"/>
+      <c r="B333" s="15"/>
     </row>
     <row r="334">
-      <c r="B334" s="14"/>
+      <c r="B334" s="15"/>
     </row>
     <row r="335">
-      <c r="B335" s="14"/>
+      <c r="B335" s="15"/>
     </row>
     <row r="336">
-      <c r="B336" s="14"/>
+      <c r="B336" s="15"/>
     </row>
     <row r="337">
-      <c r="B337" s="14"/>
+      <c r="B337" s="15"/>
     </row>
     <row r="338">
-      <c r="B338" s="14"/>
+      <c r="B338" s="15"/>
     </row>
     <row r="339">
-      <c r="B339" s="14"/>
+      <c r="B339" s="15"/>
     </row>
     <row r="340">
-      <c r="B340" s="14"/>
+      <c r="B340" s="15"/>
     </row>
     <row r="341">
-      <c r="B341" s="14"/>
+      <c r="B341" s="15"/>
     </row>
     <row r="342">
-      <c r="B342" s="14"/>
+      <c r="B342" s="15"/>
     </row>
     <row r="343">
-      <c r="B343" s="14"/>
+      <c r="B343" s="15"/>
     </row>
     <row r="344">
-      <c r="B344" s="14"/>
+      <c r="B344" s="15"/>
     </row>
     <row r="345">
-      <c r="B345" s="14"/>
+      <c r="B345" s="15"/>
     </row>
     <row r="346">
-      <c r="B346" s="14"/>
+      <c r="B346" s="15"/>
     </row>
     <row r="347">
-      <c r="B347" s="14"/>
+      <c r="B347" s="15"/>
     </row>
     <row r="348">
-      <c r="B348" s="14"/>
+      <c r="B348" s="15"/>
     </row>
     <row r="349">
-      <c r="B349" s="14"/>
+      <c r="B349" s="15"/>
     </row>
     <row r="350">
-      <c r="B350" s="14"/>
+      <c r="B350" s="15"/>
     </row>
     <row r="351">
-      <c r="B351" s="14"/>
+      <c r="B351" s="15"/>
     </row>
     <row r="352">
-      <c r="B352" s="14"/>
+      <c r="B352" s="15"/>
     </row>
     <row r="353">
-      <c r="B353" s="14"/>
+      <c r="B353" s="15"/>
     </row>
     <row r="354">
-      <c r="B354" s="14"/>
+      <c r="B354" s="15"/>
     </row>
     <row r="355">
-      <c r="B355" s="14"/>
+      <c r="B355" s="15"/>
     </row>
     <row r="356">
-      <c r="B356" s="14"/>
+      <c r="B356" s="15"/>
     </row>
     <row r="357">
-      <c r="B357" s="14"/>
+      <c r="B357" s="15"/>
     </row>
     <row r="358">
-      <c r="B358" s="14"/>
+      <c r="B358" s="15"/>
     </row>
     <row r="359">
-      <c r="B359" s="14"/>
+      <c r="B359" s="15"/>
     </row>
     <row r="360">
-      <c r="B360" s="14"/>
+      <c r="B360" s="15"/>
     </row>
     <row r="361">
-      <c r="B361" s="14"/>
+      <c r="B361" s="15"/>
     </row>
     <row r="362">
-      <c r="B362" s="14"/>
+      <c r="B362" s="15"/>
     </row>
     <row r="363">
-      <c r="B363" s="14"/>
+      <c r="B363" s="15"/>
     </row>
     <row r="364">
-      <c r="B364" s="14"/>
+      <c r="B364" s="15"/>
     </row>
     <row r="365">
-      <c r="B365" s="14"/>
+      <c r="B365" s="15"/>
     </row>
     <row r="366">
-      <c r="B366" s="14"/>
+      <c r="B366" s="15"/>
     </row>
     <row r="367">
-      <c r="B367" s="14"/>
+      <c r="B367" s="15"/>
     </row>
     <row r="368">
-      <c r="B368" s="14"/>
+      <c r="B368" s="15"/>
     </row>
     <row r="369">
-      <c r="B369" s="14"/>
+      <c r="B369" s="15"/>
     </row>
     <row r="370">
-      <c r="B370" s="14"/>
+      <c r="B370" s="15"/>
     </row>
     <row r="371">
-      <c r="B371" s="14"/>
+      <c r="B371" s="15"/>
     </row>
     <row r="372">
-      <c r="B372" s="14"/>
+      <c r="B372" s="15"/>
     </row>
     <row r="373">
-      <c r="B373" s="14"/>
+      <c r="B373" s="15"/>
     </row>
     <row r="374">
-      <c r="B374" s="14"/>
+      <c r="B374" s="15"/>
     </row>
     <row r="375">
-      <c r="B375" s="14"/>
+      <c r="B375" s="15"/>
     </row>
     <row r="376">
-      <c r="B376" s="14"/>
+      <c r="B376" s="15"/>
     </row>
     <row r="377">
-      <c r="B377" s="14"/>
+      <c r="B377" s="15"/>
     </row>
     <row r="378">
-      <c r="B378" s="14"/>
+      <c r="B378" s="15"/>
     </row>
     <row r="379">
-      <c r="B379" s="14"/>
+      <c r="B379" s="15"/>
     </row>
     <row r="380">
-      <c r="B380" s="14"/>
+      <c r="B380" s="15"/>
     </row>
     <row r="381">
-      <c r="B381" s="14"/>
+      <c r="B381" s="15"/>
     </row>
     <row r="382">
-      <c r="B382" s="14"/>
+      <c r="B382" s="15"/>
     </row>
     <row r="383">
-      <c r="B383" s="14"/>
+      <c r="B383" s="15"/>
     </row>
     <row r="384">
-      <c r="B384" s="14"/>
+      <c r="B384" s="15"/>
     </row>
     <row r="385">
-      <c r="B385" s="14"/>
+      <c r="B385" s="15"/>
     </row>
     <row r="386">
-      <c r="B386" s="14"/>
+      <c r="B386" s="15"/>
     </row>
     <row r="387">
-      <c r="B387" s="14"/>
+      <c r="B387" s="15"/>
     </row>
     <row r="388">
-      <c r="B388" s="14"/>
+      <c r="B388" s="15"/>
     </row>
     <row r="389">
-      <c r="B389" s="14"/>
+      <c r="B389" s="15"/>
     </row>
     <row r="390">
-      <c r="B390" s="14"/>
+      <c r="B390" s="15"/>
     </row>
     <row r="391">
-      <c r="B391" s="14"/>
+      <c r="B391" s="15"/>
     </row>
     <row r="392">
-      <c r="B392" s="14"/>
+      <c r="B392" s="15"/>
     </row>
     <row r="393">
-      <c r="B393" s="14"/>
+      <c r="B393" s="15"/>
     </row>
     <row r="394">
-      <c r="B394" s="14"/>
+      <c r="B394" s="15"/>
     </row>
     <row r="395">
-      <c r="B395" s="14"/>
+      <c r="B395" s="15"/>
     </row>
     <row r="396">
-      <c r="B396" s="14"/>
+      <c r="B396" s="15"/>
     </row>
     <row r="397">
-      <c r="B397" s="14"/>
+      <c r="B397" s="15"/>
     </row>
     <row r="398">
-      <c r="B398" s="14"/>
+      <c r="B398" s="15"/>
     </row>
     <row r="399">
-      <c r="B399" s="14"/>
+      <c r="B399" s="15"/>
     </row>
     <row r="400">
-      <c r="B400" s="14"/>
+      <c r="B400" s="15"/>
     </row>
     <row r="401">
-      <c r="B401" s="14"/>
+      <c r="B401" s="15"/>
     </row>
     <row r="402">
-      <c r="B402" s="14"/>
+      <c r="B402" s="15"/>
     </row>
     <row r="403">
-      <c r="B403" s="14"/>
+      <c r="B403" s="15"/>
     </row>
     <row r="404">
-      <c r="B404" s="14"/>
+      <c r="B404" s="15"/>
     </row>
     <row r="405">
-      <c r="B405" s="14"/>
+      <c r="B405" s="15"/>
     </row>
     <row r="406">
-      <c r="B406" s="14"/>
+      <c r="B406" s="15"/>
     </row>
     <row r="407">
-      <c r="B407" s="14"/>
+      <c r="B407" s="15"/>
     </row>
     <row r="408">
-      <c r="B408" s="14"/>
+      <c r="B408" s="15"/>
     </row>
     <row r="409">
-      <c r="B409" s="14"/>
+      <c r="B409" s="15"/>
     </row>
     <row r="410">
-      <c r="B410" s="14"/>
+      <c r="B410" s="15"/>
     </row>
     <row r="411">
-      <c r="B411" s="14"/>
+      <c r="B411" s="15"/>
     </row>
     <row r="412">
-      <c r="B412" s="14"/>
+      <c r="B412" s="15"/>
     </row>
     <row r="413">
-      <c r="B413" s="14"/>
+      <c r="B413" s="15"/>
     </row>
     <row r="414">
-      <c r="B414" s="14"/>
+      <c r="B414" s="15"/>
     </row>
     <row r="415">
-      <c r="B415" s="14"/>
+      <c r="B415" s="15"/>
     </row>
     <row r="416">
-      <c r="B416" s="14"/>
+      <c r="B416" s="15"/>
     </row>
     <row r="417">
-      <c r="B417" s="14"/>
+      <c r="B417" s="15"/>
     </row>
     <row r="418">
-      <c r="B418" s="14"/>
+      <c r="B418" s="15"/>
     </row>
     <row r="419">
-      <c r="B419" s="14"/>
+      <c r="B419" s="15"/>
     </row>
     <row r="420">
-      <c r="B420" s="14"/>
+      <c r="B420" s="15"/>
     </row>
     <row r="421">
-      <c r="B421" s="14"/>
+      <c r="B421" s="15"/>
     </row>
     <row r="422">
-      <c r="B422" s="14"/>
+      <c r="B422" s="15"/>
     </row>
     <row r="423">
-      <c r="B423" s="14"/>
+      <c r="B423" s="15"/>
     </row>
     <row r="424">
-      <c r="B424" s="14"/>
+      <c r="B424" s="15"/>
     </row>
     <row r="425">
-      <c r="B425" s="14"/>
+      <c r="B425" s="15"/>
     </row>
     <row r="426">
-      <c r="B426" s="14"/>
+      <c r="B426" s="15"/>
     </row>
     <row r="427">
-      <c r="B427" s="14"/>
+      <c r="B427" s="15"/>
     </row>
     <row r="428">
-      <c r="B428" s="14"/>
+      <c r="B428" s="15"/>
     </row>
     <row r="429">
-      <c r="B429" s="14"/>
+      <c r="B429" s="15"/>
     </row>
     <row r="430">
-      <c r="B430" s="14"/>
+      <c r="B430" s="15"/>
     </row>
     <row r="431">
-      <c r="B431" s="14"/>
+      <c r="B431" s="15"/>
     </row>
     <row r="432">
-      <c r="B432" s="14"/>
+      <c r="B432" s="15"/>
     </row>
     <row r="433">
-      <c r="B433" s="14"/>
+      <c r="B433" s="15"/>
     </row>
     <row r="434">
-      <c r="B434" s="14"/>
+      <c r="B434" s="15"/>
     </row>
     <row r="435">
-      <c r="B435" s="14"/>
+      <c r="B435" s="15"/>
     </row>
     <row r="436">
-      <c r="B436" s="14"/>
+      <c r="B436" s="15"/>
     </row>
     <row r="437">
-      <c r="B437" s="14"/>
+      <c r="B437" s="15"/>
     </row>
     <row r="438">
-      <c r="B438" s="14"/>
+      <c r="B438" s="15"/>
     </row>
     <row r="439">
-      <c r="B439" s="14"/>
+      <c r="B439" s="15"/>
     </row>
     <row r="440">
-      <c r="B440" s="14"/>
+      <c r="B440" s="15"/>
     </row>
     <row r="441">
-      <c r="B441" s="14"/>
+      <c r="B441" s="15"/>
     </row>
     <row r="442">
-      <c r="B442" s="14"/>
+      <c r="B442" s="15"/>
     </row>
     <row r="443">
-      <c r="B443" s="14"/>
+      <c r="B443" s="15"/>
     </row>
     <row r="444">
-      <c r="B444" s="14"/>
+      <c r="B444" s="15"/>
     </row>
     <row r="445">
-      <c r="B445" s="14"/>
+      <c r="B445" s="15"/>
     </row>
     <row r="446">
-      <c r="B446" s="14"/>
+      <c r="B446" s="15"/>
     </row>
     <row r="447">
-      <c r="B447" s="14"/>
+      <c r="B447" s="15"/>
     </row>
     <row r="448">
-      <c r="B448" s="14"/>
+      <c r="B448" s="15"/>
     </row>
     <row r="449">
-      <c r="B449" s="14"/>
+      <c r="B449" s="15"/>
     </row>
     <row r="450">
-      <c r="B450" s="14"/>
+      <c r="B450" s="15"/>
     </row>
     <row r="451">
-      <c r="B451" s="14"/>
+      <c r="B451" s="15"/>
     </row>
     <row r="452">
-      <c r="B452" s="14"/>
+      <c r="B452" s="15"/>
     </row>
     <row r="453">
-      <c r="B453" s="14"/>
+      <c r="B453" s="15"/>
     </row>
     <row r="454">
-      <c r="B454" s="14"/>
+      <c r="B454" s="15"/>
     </row>
     <row r="455">
-      <c r="B455" s="14"/>
+      <c r="B455" s="15"/>
     </row>
     <row r="456">
-      <c r="B456" s="14"/>
+      <c r="B456" s="15"/>
     </row>
     <row r="457">
-      <c r="B457" s="14"/>
+      <c r="B457" s="15"/>
     </row>
     <row r="458">
-      <c r="B458" s="14"/>
+      <c r="B458" s="15"/>
     </row>
     <row r="459">
-      <c r="B459" s="14"/>
+      <c r="B459" s="15"/>
     </row>
     <row r="460">
-      <c r="B460" s="14"/>
+      <c r="B460" s="15"/>
     </row>
     <row r="461">
-      <c r="B461" s="14"/>
+      <c r="B461" s="15"/>
     </row>
     <row r="462">
-      <c r="B462" s="14"/>
+      <c r="B462" s="15"/>
     </row>
     <row r="463">
-      <c r="B463" s="14"/>
+      <c r="B463" s="15"/>
     </row>
     <row r="464">
-      <c r="B464" s="14"/>
+      <c r="B464" s="15"/>
     </row>
     <row r="465">
-      <c r="B465" s="14"/>
+      <c r="B465" s="15"/>
     </row>
     <row r="466">
-      <c r="B466" s="14"/>
+      <c r="B466" s="15"/>
     </row>
     <row r="467">
-      <c r="B467" s="14"/>
+      <c r="B467" s="15"/>
     </row>
     <row r="468">
-      <c r="B468" s="14"/>
+      <c r="B468" s="15"/>
     </row>
     <row r="469">
-      <c r="B469" s="14"/>
+      <c r="B469" s="15"/>
     </row>
     <row r="470">
-      <c r="B470" s="14"/>
+      <c r="B470" s="15"/>
     </row>
     <row r="471">
-      <c r="B471" s="14"/>
+      <c r="B471" s="15"/>
     </row>
     <row r="472">
-      <c r="B472" s="14"/>
+      <c r="B472" s="15"/>
     </row>
     <row r="473">
-      <c r="B473" s="14"/>
+      <c r="B473" s="15"/>
     </row>
     <row r="474">
-      <c r="B474" s="14"/>
+      <c r="B474" s="15"/>
     </row>
     <row r="475">
-      <c r="B475" s="14"/>
+      <c r="B475" s="15"/>
     </row>
     <row r="476">
-      <c r="B476" s="14"/>
+      <c r="B476" s="15"/>
     </row>
     <row r="477">
-      <c r="B477" s="14"/>
+      <c r="B477" s="15"/>
     </row>
     <row r="478">
-      <c r="B478" s="14"/>
+      <c r="B478" s="15"/>
     </row>
     <row r="479">
-      <c r="B479" s="14"/>
+      <c r="B479" s="15"/>
     </row>
     <row r="480">
-      <c r="B480" s="14"/>
+      <c r="B480" s="15"/>
     </row>
     <row r="481">
-      <c r="B481" s="14"/>
+      <c r="B481" s="15"/>
     </row>
     <row r="482">
-      <c r="B482" s="14"/>
+      <c r="B482" s="15"/>
     </row>
     <row r="483">
-      <c r="B483" s="14"/>
+      <c r="B483" s="15"/>
     </row>
     <row r="484">
-      <c r="B484" s="14"/>
+      <c r="B484" s="15"/>
     </row>
     <row r="485">
-      <c r="B485" s="14"/>
+      <c r="B485" s="15"/>
     </row>
     <row r="486">
-      <c r="B486" s="14"/>
+      <c r="B486" s="15"/>
     </row>
     <row r="487">
-      <c r="B487" s="14"/>
+      <c r="B487" s="15"/>
     </row>
     <row r="488">
-      <c r="B488" s="14"/>
+      <c r="B488" s="15"/>
     </row>
     <row r="489">
-      <c r="B489" s="14"/>
+      <c r="B489" s="15"/>
     </row>
     <row r="490">
-      <c r="B490" s="14"/>
+      <c r="B490" s="15"/>
     </row>
     <row r="491">
-      <c r="B491" s="14"/>
+      <c r="B491" s="15"/>
     </row>
     <row r="492">
-      <c r="B492" s="14"/>
+      <c r="B492" s="15"/>
     </row>
     <row r="493">
-      <c r="B493" s="14"/>
+      <c r="B493" s="15"/>
     </row>
     <row r="494">
-      <c r="B494" s="14"/>
+      <c r="B494" s="15"/>
     </row>
     <row r="495">
-      <c r="B495" s="14"/>
+      <c r="B495" s="15"/>
     </row>
     <row r="496">
-      <c r="B496" s="14"/>
+      <c r="B496" s="15"/>
     </row>
     <row r="497">
-      <c r="B497" s="14"/>
+      <c r="B497" s="15"/>
     </row>
     <row r="498">
-      <c r="B498" s="14"/>
+      <c r="B498" s="15"/>
     </row>
     <row r="499">
-      <c r="B499" s="14"/>
+      <c r="B499" s="15"/>
     </row>
     <row r="500">
-      <c r="B500" s="14"/>
+      <c r="B500" s="15"/>
     </row>
     <row r="501">
-      <c r="B501" s="14"/>
+      <c r="B501" s="15"/>
     </row>
     <row r="502">
-      <c r="B502" s="14"/>
+      <c r="B502" s="15"/>
     </row>
     <row r="503">
-      <c r="B503" s="14"/>
+      <c r="B503" s="15"/>
     </row>
     <row r="504">
-      <c r="B504" s="14"/>
+      <c r="B504" s="15"/>
     </row>
     <row r="505">
-      <c r="B505" s="14"/>
+      <c r="B505" s="15"/>
     </row>
     <row r="506">
-      <c r="B506" s="14"/>
+      <c r="B506" s="15"/>
     </row>
     <row r="507">
-      <c r="B507" s="14"/>
+      <c r="B507" s="15"/>
     </row>
     <row r="508">
-      <c r="B508" s="14"/>
+      <c r="B508" s="15"/>
     </row>
     <row r="509">
-      <c r="B509" s="14"/>
+      <c r="B509" s="15"/>
     </row>
     <row r="510">
-      <c r="B510" s="14"/>
+      <c r="B510" s="15"/>
     </row>
     <row r="511">
-      <c r="B511" s="14"/>
+      <c r="B511" s="15"/>
     </row>
     <row r="512">
-      <c r="B512" s="14"/>
+      <c r="B512" s="15"/>
     </row>
     <row r="513">
-      <c r="B513" s="14"/>
+      <c r="B513" s="15"/>
     </row>
     <row r="514">
-      <c r="B514" s="14"/>
+      <c r="B514" s="15"/>
     </row>
     <row r="515">
-      <c r="B515" s="14"/>
+      <c r="B515" s="15"/>
     </row>
     <row r="516">
-      <c r="B516" s="14"/>
+      <c r="B516" s="15"/>
     </row>
     <row r="517">
-      <c r="B517" s="14"/>
+      <c r="B517" s="15"/>
     </row>
     <row r="518">
-      <c r="B518" s="14"/>
+      <c r="B518" s="15"/>
     </row>
     <row r="519">
-      <c r="B519" s="14"/>
+      <c r="B519" s="15"/>
     </row>
     <row r="520">
-      <c r="B520" s="14"/>
+      <c r="B520" s="15"/>
     </row>
     <row r="521">
-      <c r="B521" s="14"/>
+      <c r="B521" s="15"/>
     </row>
     <row r="522">
-      <c r="B522" s="14"/>
+      <c r="B522" s="15"/>
     </row>
     <row r="523">
-      <c r="B523" s="14"/>
+      <c r="B523" s="15"/>
     </row>
     <row r="524">
-      <c r="B524" s="14"/>
+      <c r="B524" s="15"/>
     </row>
     <row r="525">
-      <c r="B525" s="14"/>
+      <c r="B525" s="15"/>
     </row>
     <row r="526">
-      <c r="B526" s="14"/>
+      <c r="B526" s="15"/>
     </row>
     <row r="527">
-      <c r="B527" s="14"/>
+      <c r="B527" s="15"/>
     </row>
     <row r="528">
-      <c r="B528" s="14"/>
+      <c r="B528" s="15"/>
     </row>
     <row r="529">
-      <c r="B529" s="14"/>
+      <c r="B529" s="15"/>
     </row>
     <row r="530">
-      <c r="B530" s="14"/>
+      <c r="B530" s="15"/>
     </row>
     <row r="531">
-      <c r="B531" s="14"/>
+      <c r="B531" s="15"/>
     </row>
     <row r="532">
-      <c r="B532" s="14"/>
+      <c r="B532" s="15"/>
     </row>
     <row r="533">
-      <c r="B533" s="14"/>
+      <c r="B533" s="15"/>
     </row>
     <row r="534">
-      <c r="B534" s="14"/>
+      <c r="B534" s="15"/>
     </row>
     <row r="535">
-      <c r="B535" s="14"/>
+      <c r="B535" s="15"/>
     </row>
     <row r="536">
-      <c r="B536" s="14"/>
+      <c r="B536" s="15"/>
     </row>
     <row r="537">
-      <c r="B537" s="14"/>
+      <c r="B537" s="15"/>
     </row>
     <row r="538">
-      <c r="B538" s="14"/>
+      <c r="B538" s="15"/>
     </row>
     <row r="539">
-      <c r="B539" s="14"/>
+      <c r="B539" s="15"/>
     </row>
     <row r="540">
-      <c r="B540" s="14"/>
+      <c r="B540" s="15"/>
     </row>
     <row r="541">
-      <c r="B541" s="14"/>
+      <c r="B541" s="15"/>
     </row>
     <row r="542">
-      <c r="B542" s="14"/>
+      <c r="B542" s="15"/>
     </row>
     <row r="543">
-      <c r="B543" s="14"/>
+      <c r="B543" s="15"/>
     </row>
     <row r="544">
-      <c r="B544" s="14"/>
+      <c r="B544" s="15"/>
     </row>
     <row r="545">
-      <c r="B545" s="14"/>
+      <c r="B545" s="15"/>
     </row>
     <row r="546">
-      <c r="B546" s="14"/>
+      <c r="B546" s="15"/>
     </row>
     <row r="547">
-      <c r="B547" s="14"/>
+      <c r="B547" s="15"/>
     </row>
     <row r="548">
-      <c r="B548" s="14"/>
+      <c r="B548" s="15"/>
     </row>
     <row r="549">
-      <c r="B549" s="14"/>
+      <c r="B549" s="15"/>
     </row>
     <row r="550">
-      <c r="B550" s="14"/>
+      <c r="B550" s="15"/>
     </row>
     <row r="551">
-      <c r="B551" s="14"/>
+      <c r="B551" s="15"/>
     </row>
     <row r="552">
-      <c r="B552" s="14"/>
+      <c r="B552" s="15"/>
     </row>
     <row r="553">
-      <c r="B553" s="14"/>
+      <c r="B553" s="15"/>
     </row>
     <row r="554">
-      <c r="B554" s="14"/>
+      <c r="B554" s="15"/>
     </row>
     <row r="555">
-      <c r="B555" s="14"/>
+      <c r="B555" s="15"/>
     </row>
     <row r="556">
-      <c r="B556" s="14"/>
+      <c r="B556" s="15"/>
     </row>
     <row r="557">
-      <c r="B557" s="14"/>
+      <c r="B557" s="15"/>
     </row>
     <row r="558">
-      <c r="B558" s="14"/>
+      <c r="B558" s="15"/>
     </row>
     <row r="559">
-      <c r="B559" s="14"/>
+      <c r="B559" s="15"/>
     </row>
     <row r="560">
-      <c r="B560" s="14"/>
+      <c r="B560" s="15"/>
     </row>
     <row r="561">
-      <c r="B561" s="14"/>
+      <c r="B561" s="15"/>
     </row>
     <row r="562">
-      <c r="B562" s="14"/>
+      <c r="B562" s="15"/>
     </row>
     <row r="563">
-      <c r="B563" s="14"/>
+      <c r="B563" s="15"/>
     </row>
     <row r="564">
-      <c r="B564" s="14"/>
+      <c r="B564" s="15"/>
     </row>
     <row r="565">
-      <c r="B565" s="14"/>
+      <c r="B565" s="15"/>
     </row>
     <row r="566">
-      <c r="B566" s="14"/>
+      <c r="B566" s="15"/>
     </row>
     <row r="567">
-      <c r="B567" s="14"/>
+      <c r="B567" s="15"/>
     </row>
     <row r="568">
-      <c r="B568" s="14"/>
+      <c r="B568" s="15"/>
     </row>
     <row r="569">
-      <c r="B569" s="14"/>
+      <c r="B569" s="15"/>
     </row>
     <row r="570">
-      <c r="B570" s="14"/>
+      <c r="B570" s="15"/>
     </row>
     <row r="571">
-      <c r="B571" s="14"/>
+      <c r="B571" s="15"/>
     </row>
     <row r="572">
-      <c r="B572" s="14"/>
+      <c r="B572" s="15"/>
     </row>
     <row r="573">
-      <c r="B573" s="14"/>
+      <c r="B573" s="15"/>
     </row>
     <row r="574">
-      <c r="B574" s="14"/>
+      <c r="B574" s="15"/>
     </row>
     <row r="575">
-      <c r="B575" s="14"/>
+      <c r="B575" s="15"/>
     </row>
     <row r="576">
-      <c r="B576" s="14"/>
+      <c r="B576" s="15"/>
     </row>
     <row r="577">
-      <c r="B577" s="14"/>
+      <c r="B577" s="15"/>
     </row>
     <row r="578">
-      <c r="B578" s="14"/>
+      <c r="B578" s="15"/>
     </row>
     <row r="579">
-      <c r="B579" s="14"/>
+      <c r="B579" s="15"/>
     </row>
     <row r="580">
-      <c r="B580" s="14"/>
+      <c r="B580" s="15"/>
     </row>
     <row r="581">
-      <c r="B581" s="14"/>
+      <c r="B581" s="15"/>
     </row>
     <row r="582">
-      <c r="B582" s="14"/>
+      <c r="B582" s="15"/>
     </row>
     <row r="583">
-      <c r="B583" s="14"/>
+      <c r="B583" s="15"/>
     </row>
     <row r="584">
-      <c r="B584" s="14"/>
+      <c r="B584" s="15"/>
     </row>
     <row r="585">
-      <c r="B585" s="14"/>
+      <c r="B585" s="15"/>
     </row>
     <row r="586">
-      <c r="B586" s="14"/>
+      <c r="B586" s="15"/>
     </row>
     <row r="587">
-      <c r="B587" s="14"/>
+      <c r="B587" s="15"/>
     </row>
     <row r="588">
-      <c r="B588" s="14"/>
+      <c r="B588" s="15"/>
     </row>
     <row r="589">
-      <c r="B589" s="14"/>
+      <c r="B589" s="15"/>
     </row>
     <row r="590">
-      <c r="B590" s="14"/>
+      <c r="B590" s="15"/>
     </row>
     <row r="591">
-      <c r="B591" s="14"/>
+      <c r="B591" s="15"/>
     </row>
     <row r="592">
-      <c r="B592" s="14"/>
+      <c r="B592" s="15"/>
     </row>
     <row r="593">
-      <c r="B593" s="14"/>
+      <c r="B593" s="15"/>
     </row>
     <row r="594">
-      <c r="B594" s="14"/>
+      <c r="B594" s="15"/>
     </row>
     <row r="595">
-      <c r="B595" s="14"/>
+      <c r="B595" s="15"/>
     </row>
     <row r="596">
-      <c r="B596" s="14"/>
+      <c r="B596" s="15"/>
     </row>
     <row r="597">
-      <c r="B597" s="14"/>
+      <c r="B597" s="15"/>
     </row>
     <row r="598">
-      <c r="B598" s="14"/>
+      <c r="B598" s="15"/>
     </row>
     <row r="599">
-      <c r="B599" s="14"/>
+      <c r="B599" s="15"/>
     </row>
     <row r="600">
-      <c r="B600" s="14"/>
+      <c r="B600" s="15"/>
     </row>
     <row r="601">
-      <c r="B601" s="14"/>
+      <c r="B601" s="15"/>
     </row>
     <row r="602">
-      <c r="B602" s="14"/>
+      <c r="B602" s="15"/>
     </row>
     <row r="603">
-      <c r="B603" s="14"/>
+      <c r="B603" s="15"/>
     </row>
     <row r="604">
-      <c r="B604" s="14"/>
+      <c r="B604" s="15"/>
     </row>
     <row r="605">
-      <c r="B605" s="14"/>
+      <c r="B605" s="15"/>
     </row>
     <row r="606">
-      <c r="B606" s="14"/>
+      <c r="B606" s="15"/>
     </row>
     <row r="607">
-      <c r="B607" s="14"/>
+      <c r="B607" s="15"/>
     </row>
     <row r="608">
-      <c r="B608" s="14"/>
+      <c r="B608" s="15"/>
     </row>
     <row r="609">
-      <c r="B609" s="14"/>
+      <c r="B609" s="15"/>
     </row>
     <row r="610">
-      <c r="B610" s="14"/>
+      <c r="B610" s="15"/>
     </row>
     <row r="611">
-      <c r="B611" s="14"/>
+      <c r="B611" s="15"/>
     </row>
     <row r="612">
-      <c r="B612" s="14"/>
+      <c r="B612" s="15"/>
     </row>
     <row r="613">
-      <c r="B613" s="14"/>
+      <c r="B613" s="15"/>
     </row>
     <row r="614">
-      <c r="B614" s="14"/>
+      <c r="B614" s="15"/>
     </row>
     <row r="615">
-      <c r="B615" s="14"/>
+      <c r="B615" s="15"/>
     </row>
     <row r="616">
-      <c r="B616" s="14"/>
+      <c r="B616" s="15"/>
     </row>
     <row r="617">
-      <c r="B617" s="14"/>
+      <c r="B617" s="15"/>
     </row>
     <row r="618">
-      <c r="B618" s="14"/>
+      <c r="B618" s="15"/>
     </row>
     <row r="619">
-      <c r="B619" s="14"/>
+      <c r="B619" s="15"/>
     </row>
     <row r="620">
-      <c r="B620" s="14"/>
+      <c r="B620" s="15"/>
     </row>
     <row r="621">
-      <c r="B621" s="14"/>
+      <c r="B621" s="15"/>
     </row>
     <row r="622">
-      <c r="B622" s="14"/>
+      <c r="B622" s="15"/>
     </row>
     <row r="623">
-      <c r="B623" s="14"/>
+      <c r="B623" s="15"/>
     </row>
     <row r="624">
-      <c r="B624" s="14"/>
+      <c r="B624" s="15"/>
     </row>
     <row r="625">
-      <c r="B625" s="14"/>
+      <c r="B625" s="15"/>
     </row>
     <row r="626">
-      <c r="B626" s="14"/>
+      <c r="B626" s="15"/>
     </row>
     <row r="627">
-      <c r="B627" s="14"/>
+      <c r="B627" s="15"/>
     </row>
     <row r="628">
-      <c r="B628" s="14"/>
+      <c r="B628" s="15"/>
     </row>
     <row r="629">
-      <c r="B629" s="14"/>
+      <c r="B629" s="15"/>
     </row>
     <row r="630">
-      <c r="B630" s="14"/>
+      <c r="B630" s="15"/>
     </row>
     <row r="631">
-      <c r="B631" s="14"/>
+      <c r="B631" s="15"/>
     </row>
     <row r="632">
-      <c r="B632" s="14"/>
+      <c r="B632" s="15"/>
     </row>
     <row r="633">
-      <c r="B633" s="14"/>
+      <c r="B633" s="15"/>
     </row>
     <row r="634">
-      <c r="B634" s="14"/>
+      <c r="B634" s="15"/>
     </row>
     <row r="635">
-      <c r="B635" s="14"/>
+      <c r="B635" s="15"/>
     </row>
     <row r="636">
-      <c r="B636" s="14"/>
+      <c r="B636" s="15"/>
     </row>
     <row r="637">
-      <c r="B637" s="14"/>
+      <c r="B637" s="15"/>
     </row>
     <row r="638">
-      <c r="B638" s="14"/>
+      <c r="B638" s="15"/>
     </row>
     <row r="639">
-      <c r="B639" s="14"/>
+      <c r="B639" s="15"/>
     </row>
     <row r="640">
-      <c r="B640" s="14"/>
+      <c r="B640" s="15"/>
     </row>
     <row r="641">
-      <c r="B641" s="14"/>
+      <c r="B641" s="15"/>
     </row>
     <row r="642">
-      <c r="B642" s="14"/>
+      <c r="B642" s="15"/>
     </row>
     <row r="643">
-      <c r="B643" s="14"/>
+      <c r="B643" s="15"/>
     </row>
     <row r="644">
-      <c r="B644" s="14"/>
+      <c r="B644" s="15"/>
     </row>
     <row r="645">
-      <c r="B645" s="14"/>
+      <c r="B645" s="15"/>
     </row>
     <row r="646">
-      <c r="B646" s="14"/>
+      <c r="B646" s="15"/>
     </row>
     <row r="647">
-      <c r="B647" s="14"/>
+      <c r="B647" s="15"/>
     </row>
     <row r="648">
-      <c r="B648" s="14"/>
+      <c r="B648" s="15"/>
     </row>
     <row r="649">
-      <c r="B649" s="14"/>
+      <c r="B649" s="15"/>
     </row>
     <row r="650">
-      <c r="B650" s="14"/>
+      <c r="B650" s="15"/>
     </row>
     <row r="651">
-      <c r="B651" s="14"/>
+      <c r="B651" s="15"/>
     </row>
     <row r="652">
-      <c r="B652" s="14"/>
+      <c r="B652" s="15"/>
     </row>
     <row r="653">
-      <c r="B653" s="14"/>
+      <c r="B653" s="15"/>
     </row>
     <row r="654">
-      <c r="B654" s="14"/>
+      <c r="B654" s="15"/>
     </row>
     <row r="655">
-      <c r="B655" s="14"/>
+      <c r="B655" s="15"/>
     </row>
     <row r="656">
-      <c r="B656" s="14"/>
+      <c r="B656" s="15"/>
     </row>
     <row r="657">
-      <c r="B657" s="14"/>
+      <c r="B657" s="15"/>
     </row>
     <row r="658">
-      <c r="B658" s="14"/>
+      <c r="B658" s="15"/>
     </row>
     <row r="659">
-      <c r="B659" s="14"/>
+      <c r="B659" s="15"/>
     </row>
     <row r="660">
-      <c r="B660" s="14"/>
+      <c r="B660" s="15"/>
     </row>
     <row r="661">
-      <c r="B661" s="14"/>
+      <c r="B661" s="15"/>
     </row>
     <row r="662">
-      <c r="B662" s="14"/>
+      <c r="B662" s="15"/>
     </row>
     <row r="663">
-      <c r="B663" s="14"/>
+      <c r="B663" s="15"/>
     </row>
     <row r="664">
-      <c r="B664" s="14"/>
+      <c r="B664" s="15"/>
     </row>
     <row r="665">
-      <c r="B665" s="14"/>
+      <c r="B665" s="15"/>
     </row>
     <row r="666">
-      <c r="B666" s="14"/>
+      <c r="B666" s="15"/>
     </row>
     <row r="667">
-      <c r="B667" s="14"/>
+      <c r="B667" s="15"/>
     </row>
     <row r="668">
-      <c r="B668" s="14"/>
+      <c r="B668" s="15"/>
     </row>
     <row r="669">
-      <c r="B669" s="14"/>
+      <c r="B669" s="15"/>
     </row>
     <row r="670">
-      <c r="B670" s="14"/>
+      <c r="B670" s="15"/>
     </row>
     <row r="671">
-      <c r="B671" s="14"/>
+      <c r="B671" s="15"/>
     </row>
     <row r="672">
-      <c r="B672" s="14"/>
+      <c r="B672" s="15"/>
     </row>
     <row r="673">
-      <c r="B673" s="14"/>
+      <c r="B673" s="15"/>
     </row>
     <row r="674">
-      <c r="B674" s="14"/>
+      <c r="B674" s="15"/>
     </row>
     <row r="675">
-      <c r="B675" s="14"/>
+      <c r="B675" s="15"/>
     </row>
     <row r="676">
-      <c r="B676" s="14"/>
+      <c r="B676" s="15"/>
     </row>
     <row r="677">
-      <c r="B677" s="14"/>
+      <c r="B677" s="15"/>
     </row>
     <row r="678">
-      <c r="B678" s="14"/>
+      <c r="B678" s="15"/>
     </row>
     <row r="679">
-      <c r="B679" s="14"/>
+      <c r="B679" s="15"/>
     </row>
     <row r="680">
-      <c r="B680" s="14"/>
+      <c r="B680" s="15"/>
     </row>
     <row r="681">
-      <c r="B681" s="14"/>
+      <c r="B681" s="15"/>
     </row>
     <row r="682">
-      <c r="B682" s="14"/>
+      <c r="B682" s="15"/>
     </row>
     <row r="683">
-      <c r="B683" s="14"/>
+      <c r="B683" s="15"/>
     </row>
     <row r="684">
-      <c r="B684" s="14"/>
+      <c r="B684" s="15"/>
     </row>
     <row r="685">
-      <c r="B685" s="14"/>
+      <c r="B685" s="15"/>
     </row>
     <row r="686">
-      <c r="B686" s="14"/>
+      <c r="B686" s="15"/>
     </row>
     <row r="687">
-      <c r="B687" s="14"/>
+      <c r="B687" s="15"/>
     </row>
     <row r="688">
-      <c r="B688" s="14"/>
+      <c r="B688" s="15"/>
     </row>
     <row r="689">
-      <c r="B689" s="14"/>
+      <c r="B689" s="15"/>
     </row>
     <row r="690">
-      <c r="B690" s="14"/>
+      <c r="B690" s="15"/>
     </row>
     <row r="691">
-      <c r="B691" s="14"/>
+      <c r="B691" s="15"/>
     </row>
     <row r="692">
-      <c r="B692" s="14"/>
+      <c r="B692" s="15"/>
     </row>
     <row r="693">
-      <c r="B693" s="14"/>
+      <c r="B693" s="15"/>
     </row>
     <row r="694">
-      <c r="B694" s="14"/>
+      <c r="B694" s="15"/>
     </row>
     <row r="695">
-      <c r="B695" s="14"/>
+      <c r="B695" s="15"/>
     </row>
     <row r="696">
-      <c r="B696" s="14"/>
+      <c r="B696" s="15"/>
     </row>
     <row r="697">
-      <c r="B697" s="14"/>
+      <c r="B697" s="15"/>
     </row>
     <row r="698">
-      <c r="B698" s="14"/>
+      <c r="B698" s="15"/>
     </row>
     <row r="699">
-      <c r="B699" s="14"/>
+      <c r="B699" s="15"/>
     </row>
     <row r="700">
-      <c r="B700" s="14"/>
+      <c r="B700" s="15"/>
     </row>
     <row r="701">
-      <c r="B701" s="14"/>
+      <c r="B701" s="15"/>
     </row>
     <row r="702">
-      <c r="B702" s="14"/>
+      <c r="B702" s="15"/>
     </row>
     <row r="703">
-      <c r="B703" s="14"/>
+      <c r="B703" s="15"/>
     </row>
     <row r="704">
-      <c r="B704" s="14"/>
+      <c r="B704" s="15"/>
     </row>
     <row r="705">
-      <c r="B705" s="14"/>
+      <c r="B705" s="15"/>
     </row>
     <row r="706">
-      <c r="B706" s="14"/>
+      <c r="B706" s="15"/>
     </row>
     <row r="707">
-      <c r="B707" s="14"/>
+      <c r="B707" s="15"/>
     </row>
     <row r="708">
-      <c r="B708" s="14"/>
+      <c r="B708" s="15"/>
     </row>
     <row r="709">
-      <c r="B709" s="14"/>
+      <c r="B709" s="15"/>
     </row>
     <row r="710">
-      <c r="B710" s="14"/>
+      <c r="B710" s="15"/>
     </row>
     <row r="711">
-      <c r="B711" s="14"/>
+      <c r="B711" s="15"/>
     </row>
     <row r="712">
-      <c r="B712" s="14"/>
+      <c r="B712" s="15"/>
     </row>
     <row r="713">
-      <c r="B713" s="14"/>
+      <c r="B713" s="15"/>
     </row>
     <row r="714">
-      <c r="B714" s="14"/>
+      <c r="B714" s="15"/>
     </row>
     <row r="715">
-      <c r="B715" s="14"/>
+      <c r="B715" s="15"/>
     </row>
     <row r="716">
-      <c r="B716" s="14"/>
+      <c r="B716" s="15"/>
     </row>
     <row r="717">
-      <c r="B717" s="14"/>
+      <c r="B717" s="15"/>
     </row>
     <row r="718">
-      <c r="B718" s="14"/>
+      <c r="B718" s="15"/>
     </row>
     <row r="719">
-      <c r="B719" s="14"/>
+      <c r="B719" s="15"/>
     </row>
     <row r="720">
-      <c r="B720" s="14"/>
+      <c r="B720" s="15"/>
     </row>
     <row r="721">
-      <c r="B721" s="14"/>
+      <c r="B721" s="15"/>
     </row>
     <row r="722">
-      <c r="B722" s="14"/>
+      <c r="B722" s="15"/>
     </row>
     <row r="723">
-      <c r="B723" s="14"/>
+      <c r="B723" s="15"/>
     </row>
     <row r="724">
-      <c r="B724" s="14"/>
+      <c r="B724" s="15"/>
     </row>
     <row r="725">
-      <c r="B725" s="14"/>
+      <c r="B725" s="15"/>
     </row>
     <row r="726">
-      <c r="B726" s="14"/>
+      <c r="B726" s="15"/>
     </row>
     <row r="727">
-      <c r="B727" s="14"/>
+      <c r="B727" s="15"/>
     </row>
     <row r="728">
-      <c r="B728" s="14"/>
+      <c r="B728" s="15"/>
     </row>
     <row r="729">
-      <c r="B729" s="14"/>
+      <c r="B729" s="15"/>
     </row>
     <row r="730">
-      <c r="B730" s="14"/>
+      <c r="B730" s="15"/>
     </row>
     <row r="731">
-      <c r="B731" s="14"/>
+      <c r="B731" s="15"/>
     </row>
     <row r="732">
-      <c r="B732" s="14"/>
+      <c r="B732" s="15"/>
     </row>
     <row r="733">
-      <c r="B733" s="14"/>
+      <c r="B733" s="15"/>
     </row>
     <row r="734">
-      <c r="B734" s="14"/>
+      <c r="B734" s="15"/>
     </row>
     <row r="735">
-      <c r="B735" s="14"/>
+      <c r="B735" s="15"/>
     </row>
     <row r="736">
-      <c r="B736" s="14"/>
+      <c r="B736" s="15"/>
     </row>
     <row r="737">
-      <c r="B737" s="14"/>
+      <c r="B737" s="15"/>
     </row>
     <row r="738">
-      <c r="B738" s="14"/>
+      <c r="B738" s="15"/>
     </row>
     <row r="739">
-      <c r="B739" s="14"/>
+      <c r="B739" s="15"/>
     </row>
     <row r="740">
-      <c r="B740" s="14"/>
+      <c r="B740" s="15"/>
     </row>
     <row r="741">
-      <c r="B741" s="14"/>
+      <c r="B741" s="15"/>
     </row>
     <row r="742">
-      <c r="B742" s="14"/>
+      <c r="B742" s="15"/>
     </row>
     <row r="743">
-      <c r="B743" s="14"/>
+      <c r="B743" s="15"/>
     </row>
     <row r="744">
-      <c r="B744" s="14"/>
+      <c r="B744" s="15"/>
     </row>
     <row r="745">
-      <c r="B745" s="14"/>
+      <c r="B745" s="15"/>
     </row>
     <row r="746">
-      <c r="B746" s="14"/>
+      <c r="B746" s="15"/>
     </row>
     <row r="747">
-      <c r="B747" s="14"/>
+      <c r="B747" s="15"/>
     </row>
     <row r="748">
-      <c r="B748" s="14"/>
+      <c r="B748" s="15"/>
     </row>
     <row r="749">
-      <c r="B749" s="14"/>
+      <c r="B749" s="15"/>
     </row>
     <row r="750">
-      <c r="B750" s="14"/>
+      <c r="B750" s="15"/>
     </row>
     <row r="751">
-      <c r="B751" s="14"/>
+      <c r="B751" s="15"/>
     </row>
     <row r="752">
-      <c r="B752" s="14"/>
+      <c r="B752" s="15"/>
     </row>
     <row r="753">
-      <c r="B753" s="14"/>
+      <c r="B753" s="15"/>
     </row>
     <row r="754">
-      <c r="B754" s="14"/>
+      <c r="B754" s="15"/>
     </row>
     <row r="755">
-      <c r="B755" s="14"/>
+      <c r="B755" s="15"/>
     </row>
     <row r="756">
-      <c r="B756" s="14"/>
+      <c r="B756" s="15"/>
     </row>
     <row r="757">
-      <c r="B757" s="14"/>
+      <c r="B757" s="15"/>
     </row>
     <row r="758">
-      <c r="B758" s="14"/>
+      <c r="B758" s="15"/>
     </row>
     <row r="759">
-      <c r="B759" s="14"/>
+      <c r="B759" s="15"/>
     </row>
     <row r="760">
-      <c r="B760" s="14"/>
+      <c r="B760" s="15"/>
     </row>
     <row r="761">
-      <c r="B761" s="14"/>
+      <c r="B761" s="15"/>
     </row>
     <row r="762">
-      <c r="B762" s="14"/>
+      <c r="B762" s="15"/>
     </row>
     <row r="763">
-      <c r="B763" s="14"/>
+      <c r="B763" s="15"/>
     </row>
     <row r="764">
-      <c r="B764" s="14"/>
+      <c r="B764" s="15"/>
     </row>
     <row r="765">
-      <c r="B765" s="14"/>
+      <c r="B765" s="15"/>
     </row>
     <row r="766">
-      <c r="B766" s="14"/>
+      <c r="B766" s="15"/>
     </row>
     <row r="767">
-      <c r="B767" s="14"/>
+      <c r="B767" s="15"/>
     </row>
     <row r="768">
-      <c r="B768" s="14"/>
+      <c r="B768" s="15"/>
     </row>
     <row r="769">
-      <c r="B769" s="14"/>
+      <c r="B769" s="15"/>
     </row>
     <row r="770">
-      <c r="B770" s="14"/>
+      <c r="B770" s="15"/>
     </row>
     <row r="771">
-      <c r="B771" s="14"/>
+      <c r="B771" s="15"/>
     </row>
     <row r="772">
-      <c r="B772" s="14"/>
+      <c r="B772" s="15"/>
     </row>
     <row r="773">
-      <c r="B773" s="14"/>
+      <c r="B773" s="15"/>
     </row>
     <row r="774">
-      <c r="B774" s="14"/>
+      <c r="B774" s="15"/>
     </row>
     <row r="775">
-      <c r="B775" s="14"/>
+      <c r="B775" s="15"/>
     </row>
     <row r="776">
-      <c r="B776" s="14"/>
+      <c r="B776" s="15"/>
     </row>
     <row r="777">
-      <c r="B777" s="14"/>
+      <c r="B777" s="15"/>
     </row>
     <row r="778">
-      <c r="B778" s="14"/>
+      <c r="B778" s="15"/>
     </row>
     <row r="779">
-      <c r="B779" s="14"/>
+      <c r="B779" s="15"/>
     </row>
     <row r="780">
-      <c r="B780" s="14"/>
+      <c r="B780" s="15"/>
     </row>
     <row r="781">
-      <c r="B781" s="14"/>
+      <c r="B781" s="15"/>
     </row>
     <row r="782">
-      <c r="B782" s="14"/>
+      <c r="B782" s="15"/>
     </row>
     <row r="783">
-      <c r="B783" s="14"/>
+      <c r="B783" s="15"/>
     </row>
     <row r="784">
-      <c r="B784" s="14"/>
+      <c r="B784" s="15"/>
     </row>
     <row r="785">
-      <c r="B785" s="14"/>
+      <c r="B785" s="15"/>
     </row>
     <row r="786">
-      <c r="B786" s="14"/>
+      <c r="B786" s="15"/>
     </row>
     <row r="787">
-      <c r="B787" s="14"/>
+      <c r="B787" s="15"/>
     </row>
     <row r="788">
-      <c r="B788" s="14"/>
+      <c r="B788" s="15"/>
     </row>
     <row r="789">
-      <c r="B789" s="14"/>
+      <c r="B789" s="15"/>
     </row>
     <row r="790">
-      <c r="B790" s="14"/>
+      <c r="B790" s="15"/>
     </row>
     <row r="791">
-      <c r="B791" s="14"/>
+      <c r="B791" s="15"/>
     </row>
     <row r="792">
-      <c r="B792" s="14"/>
+      <c r="B792" s="15"/>
     </row>
     <row r="793">
-      <c r="B793" s="14"/>
+      <c r="B793" s="15"/>
     </row>
     <row r="794">
-      <c r="B794" s="14"/>
+      <c r="B794" s="15"/>
     </row>
     <row r="795">
-      <c r="B795" s="14"/>
+      <c r="B795" s="15"/>
     </row>
     <row r="796">
-      <c r="B796" s="14"/>
+      <c r="B796" s="15"/>
     </row>
     <row r="797">
-      <c r="B797" s="14"/>
+      <c r="B797" s="15"/>
     </row>
     <row r="798">
-      <c r="B798" s="14"/>
+      <c r="B798" s="15"/>
     </row>
     <row r="799">
-      <c r="B799" s="14"/>
+      <c r="B799" s="15"/>
     </row>
     <row r="800">
-      <c r="B800" s="14"/>
+      <c r="B800" s="15"/>
     </row>
     <row r="801">
-      <c r="B801" s="14"/>
+      <c r="B801" s="15"/>
     </row>
     <row r="802">
-      <c r="B802" s="14"/>
+      <c r="B802" s="15"/>
     </row>
     <row r="803">
-      <c r="B803" s="14"/>
+      <c r="B803" s="15"/>
     </row>
     <row r="804">
-      <c r="B804" s="14"/>
+      <c r="B804" s="15"/>
     </row>
     <row r="805">
-      <c r="B805" s="14"/>
+      <c r="B805" s="15"/>
     </row>
     <row r="806">
-      <c r="B806" s="14"/>
+      <c r="B806" s="15"/>
     </row>
     <row r="807">
-      <c r="B807" s="14"/>
+      <c r="B807" s="15"/>
     </row>
     <row r="808">
-      <c r="B808" s="14"/>
+      <c r="B808" s="15"/>
     </row>
     <row r="809">
-      <c r="B809" s="14"/>
+      <c r="B809" s="15"/>
     </row>
     <row r="810">
-      <c r="B810" s="14"/>
+      <c r="B810" s="15"/>
     </row>
     <row r="811">
-      <c r="B811" s="14"/>
+      <c r="B811" s="15"/>
     </row>
     <row r="812">
-      <c r="B812" s="14"/>
+      <c r="B812" s="15"/>
     </row>
     <row r="813">
-      <c r="B813" s="14"/>
+      <c r="B813" s="15"/>
     </row>
     <row r="814">
-      <c r="B814" s="14"/>
+      <c r="B814" s="15"/>
     </row>
     <row r="815">
-      <c r="B815" s="14"/>
+      <c r="B815" s="15"/>
     </row>
     <row r="816">
-      <c r="B816" s="14"/>
+      <c r="B816" s="15"/>
     </row>
     <row r="817">
-      <c r="B817" s="14"/>
+      <c r="B817" s="15"/>
     </row>
     <row r="818">
-      <c r="B818" s="14"/>
+      <c r="B818" s="15"/>
     </row>
     <row r="819">
-      <c r="B819" s="14"/>
+      <c r="B819" s="15"/>
     </row>
     <row r="820">
-      <c r="B820" s="14"/>
+      <c r="B820" s="15"/>
     </row>
     <row r="821">
-      <c r="B821" s="14"/>
+      <c r="B821" s="15"/>
     </row>
     <row r="822">
-      <c r="B822" s="14"/>
+      <c r="B822" s="15"/>
     </row>
     <row r="823">
-      <c r="B823" s="14"/>
+      <c r="B823" s="15"/>
     </row>
     <row r="824">
-      <c r="B824" s="14"/>
+      <c r="B824" s="15"/>
     </row>
     <row r="825">
-      <c r="B825" s="14"/>
+      <c r="B825" s="15"/>
     </row>
     <row r="826">
-      <c r="B826" s="14"/>
+      <c r="B826" s="15"/>
     </row>
     <row r="827">
-      <c r="B827" s="14"/>
+      <c r="B827" s="15"/>
     </row>
     <row r="828">
-      <c r="B828" s="14"/>
+      <c r="B828" s="15"/>
     </row>
     <row r="829">
-      <c r="B829" s="14"/>
+      <c r="B829" s="15"/>
     </row>
     <row r="830">
-      <c r="B830" s="14"/>
+      <c r="B830" s="15"/>
     </row>
     <row r="831">
-      <c r="B831" s="14"/>
+      <c r="B831" s="15"/>
     </row>
     <row r="832">
-      <c r="B832" s="14"/>
+      <c r="B832" s="15"/>
     </row>
     <row r="833">
-      <c r="B833" s="14"/>
+      <c r="B833" s="15"/>
     </row>
     <row r="834">
-      <c r="B834" s="14"/>
+      <c r="B834" s="15"/>
     </row>
     <row r="835">
-      <c r="B835" s="14"/>
+      <c r="B835" s="15"/>
     </row>
     <row r="836">
-      <c r="B836" s="14"/>
+      <c r="B836" s="15"/>
     </row>
     <row r="837">
-      <c r="B837" s="14"/>
+      <c r="B837" s="15"/>
     </row>
     <row r="838">
-      <c r="B838" s="14"/>
+      <c r="B838" s="15"/>
     </row>
     <row r="839">
-      <c r="B839" s="14"/>
+      <c r="B839" s="15"/>
     </row>
     <row r="840">
-      <c r="B840" s="14"/>
+      <c r="B840" s="15"/>
     </row>
     <row r="841">
-      <c r="B841" s="14"/>
+      <c r="B841" s="15"/>
     </row>
     <row r="842">
-      <c r="B842" s="14"/>
+      <c r="B842" s="15"/>
     </row>
     <row r="843">
-      <c r="B843" s="14"/>
+      <c r="B843" s="15"/>
     </row>
     <row r="844">
-      <c r="B844" s="14"/>
+      <c r="B844" s="15"/>
     </row>
     <row r="845">
-      <c r="B845" s="14"/>
+      <c r="B845" s="15"/>
     </row>
     <row r="846">
-      <c r="B846" s="14"/>
+      <c r="B846" s="15"/>
     </row>
     <row r="847">
-      <c r="B847" s="14"/>
+      <c r="B847" s="15"/>
     </row>
     <row r="848">
-      <c r="B848" s="14"/>
+      <c r="B848" s="15"/>
     </row>
     <row r="849">
-      <c r="B849" s="14"/>
+      <c r="B849" s="15"/>
     </row>
     <row r="850">
-      <c r="B850" s="14"/>
+      <c r="B850" s="15"/>
     </row>
     <row r="851">
-      <c r="B851" s="14"/>
+      <c r="B851" s="15"/>
     </row>
     <row r="852">
-      <c r="B852" s="14"/>
+      <c r="B852" s="15"/>
     </row>
     <row r="853">
-      <c r="B853" s="14"/>
+      <c r="B853" s="15"/>
     </row>
     <row r="854">
-      <c r="B854" s="14"/>
+      <c r="B854" s="15"/>
     </row>
     <row r="855">
-      <c r="B855" s="14"/>
+      <c r="B855" s="15"/>
     </row>
     <row r="856">
-      <c r="B856" s="14"/>
+      <c r="B856" s="15"/>
     </row>
     <row r="857">
-      <c r="B857" s="14"/>
+      <c r="B857" s="15"/>
     </row>
     <row r="858">
-      <c r="B858" s="14"/>
+      <c r="B858" s="15"/>
     </row>
     <row r="859">
-      <c r="B859" s="14"/>
+      <c r="B859" s="15"/>
     </row>
     <row r="860">
-      <c r="B860" s="14"/>
+      <c r="B860" s="15"/>
     </row>
     <row r="861">
-      <c r="B861" s="14"/>
+      <c r="B861" s="15"/>
     </row>
     <row r="862">
-      <c r="B862" s="14"/>
+      <c r="B862" s="15"/>
     </row>
     <row r="863">
-      <c r="B863" s="14"/>
+      <c r="B863" s="15"/>
     </row>
     <row r="864">
-      <c r="B864" s="14"/>
+      <c r="B864" s="15"/>
     </row>
     <row r="865">
-      <c r="B865" s="14"/>
+      <c r="B865" s="15"/>
     </row>
     <row r="866">
-      <c r="B866" s="14"/>
+      <c r="B866" s="15"/>
     </row>
     <row r="867">
-      <c r="B867" s="14"/>
+      <c r="B867" s="15"/>
     </row>
     <row r="868">
-      <c r="B868" s="14"/>
+      <c r="B868" s="15"/>
     </row>
     <row r="869">
-      <c r="B869" s="14"/>
+      <c r="B869" s="15"/>
     </row>
     <row r="870">
-      <c r="B870" s="14"/>
+      <c r="B870" s="15"/>
     </row>
     <row r="871">
-      <c r="B871" s="14"/>
+      <c r="B871" s="15"/>
     </row>
     <row r="872">
-      <c r="B872" s="14"/>
+      <c r="B872" s="15"/>
     </row>
     <row r="873">
-      <c r="B873" s="14"/>
+      <c r="B873" s="15"/>
     </row>
     <row r="874">
-      <c r="B874" s="14"/>
+      <c r="B874" s="15"/>
     </row>
     <row r="875">
-      <c r="B875" s="14"/>
+      <c r="B875" s="15"/>
     </row>
     <row r="876">
-      <c r="B876" s="14"/>
+      <c r="B876" s="15"/>
     </row>
     <row r="877">
-      <c r="B877" s="14"/>
+      <c r="B877" s="15"/>
     </row>
     <row r="878">
-      <c r="B878" s="14"/>
+      <c r="B878" s="15"/>
     </row>
     <row r="879">
-      <c r="B879" s="14"/>
+      <c r="B879" s="15"/>
     </row>
     <row r="880">
-      <c r="B880" s="14"/>
+      <c r="B880" s="15"/>
     </row>
     <row r="881">
-      <c r="B881" s="14"/>
+      <c r="B881" s="15"/>
     </row>
     <row r="882">
-      <c r="B882" s="14"/>
+      <c r="B882" s="15"/>
     </row>
     <row r="883">
-      <c r="B883" s="14"/>
+      <c r="B883" s="15"/>
     </row>
     <row r="884">
-      <c r="B884" s="14"/>
+      <c r="B884" s="15"/>
     </row>
     <row r="885">
-      <c r="B885" s="14"/>
+      <c r="B885" s="15"/>
     </row>
     <row r="886">
-      <c r="B886" s="14"/>
+      <c r="B886" s="15"/>
     </row>
     <row r="887">
-      <c r="B887" s="14"/>
+      <c r="B887" s="15"/>
     </row>
     <row r="888">
-      <c r="B888" s="14"/>
+      <c r="B888" s="15"/>
     </row>
     <row r="889">
-      <c r="B889" s="14"/>
+      <c r="B889" s="15"/>
     </row>
     <row r="890">
-      <c r="B890" s="14"/>
+      <c r="B890" s="15"/>
     </row>
     <row r="891">
-      <c r="B891" s="14"/>
+      <c r="B891" s="15"/>
     </row>
     <row r="892">
-      <c r="B892" s="14"/>
+      <c r="B892" s="15"/>
     </row>
     <row r="893">
-      <c r="B893" s="14"/>
+      <c r="B893" s="15"/>
     </row>
     <row r="894">
-      <c r="B894" s="14"/>
+      <c r="B894" s="15"/>
     </row>
     <row r="895">
-      <c r="B895" s="14"/>
+      <c r="B895" s="15"/>
     </row>
     <row r="896">
-      <c r="B896" s="14"/>
+      <c r="B896" s="15"/>
     </row>
     <row r="897">
-      <c r="B897" s="14"/>
+      <c r="B897" s="15"/>
     </row>
     <row r="898">
-      <c r="B898" s="14"/>
+      <c r="B898" s="15"/>
     </row>
     <row r="899">
-      <c r="B899" s="14"/>
+      <c r="B899" s="15"/>
     </row>
     <row r="900">
-      <c r="B900" s="14"/>
+      <c r="B900" s="15"/>
     </row>
     <row r="901">
-      <c r="B901" s="14"/>
+      <c r="B901" s="15"/>
     </row>
     <row r="902">
-      <c r="B902" s="14"/>
+      <c r="B902" s="15"/>
     </row>
     <row r="903">
-      <c r="B903" s="14"/>
+      <c r="B903" s="15"/>
     </row>
     <row r="904">
-      <c r="B904" s="14"/>
+      <c r="B904" s="15"/>
     </row>
     <row r="905">
-      <c r="B905" s="14"/>
+      <c r="B905" s="15"/>
     </row>
     <row r="906">
-      <c r="B906" s="14"/>
+      <c r="B906" s="15"/>
     </row>
     <row r="907">
-      <c r="B907" s="14"/>
+      <c r="B907" s="15"/>
     </row>
     <row r="908">
-      <c r="B908" s="14"/>
+      <c r="B908" s="15"/>
     </row>
     <row r="909">
-      <c r="B909" s="14"/>
+      <c r="B909" s="15"/>
     </row>
     <row r="910">
-      <c r="B910" s="14"/>
+      <c r="B910" s="15"/>
     </row>
     <row r="911">
-      <c r="B911" s="14"/>
+      <c r="B911" s="15"/>
     </row>
     <row r="912">
-      <c r="B912" s="14"/>
+      <c r="B912" s="15"/>
     </row>
     <row r="913">
-      <c r="B913" s="14"/>
+      <c r="B913" s="15"/>
     </row>
     <row r="914">
-      <c r="B914" s="14"/>
+      <c r="B914" s="15"/>
     </row>
     <row r="915">
-      <c r="B915" s="14"/>
+      <c r="B915" s="15"/>
     </row>
     <row r="916">
-      <c r="B916" s="14"/>
+      <c r="B916" s="15"/>
     </row>
     <row r="917">
-      <c r="B917" s="14"/>
+      <c r="B917" s="15"/>
     </row>
     <row r="918">
-      <c r="B918" s="14"/>
+      <c r="B918" s="15"/>
     </row>
     <row r="919">
-      <c r="B919" s="14"/>
+      <c r="B919" s="15"/>
     </row>
     <row r="920">
-      <c r="B920" s="14"/>
+      <c r="B920" s="15"/>
     </row>
     <row r="921">
-      <c r="B921" s="14"/>
+      <c r="B921" s="15"/>
     </row>
     <row r="922">
-      <c r="B922" s="14"/>
+      <c r="B922" s="15"/>
     </row>
     <row r="923">
-      <c r="B923" s="14"/>
+      <c r="B923" s="15"/>
     </row>
     <row r="924">
-      <c r="B924" s="14"/>
+      <c r="B924" s="15"/>
     </row>
     <row r="925">
-      <c r="B925" s="14"/>
+      <c r="B925" s="15"/>
     </row>
     <row r="926">
-      <c r="B926" s="14"/>
+      <c r="B926" s="15"/>
     </row>
     <row r="927">
-      <c r="B927" s="14"/>
+      <c r="B927" s="15"/>
     </row>
     <row r="928">
-      <c r="B928" s="14"/>
+      <c r="B928" s="15"/>
     </row>
     <row r="929">
-      <c r="B929" s="14"/>
+      <c r="B929" s="15"/>
     </row>
     <row r="930">
-      <c r="B930" s="14"/>
+      <c r="B930" s="15"/>
     </row>
     <row r="931">
-      <c r="B931" s="14"/>
+      <c r="B931" s="15"/>
     </row>
     <row r="932">
-      <c r="B932" s="14"/>
+      <c r="B932" s="15"/>
     </row>
     <row r="933">
-      <c r="B933" s="14"/>
+      <c r="B933" s="15"/>
     </row>
     <row r="934">
-      <c r="B934" s="14"/>
+      <c r="B934" s="15"/>
     </row>
     <row r="935">
-      <c r="B935" s="14"/>
+      <c r="B935" s="15"/>
     </row>
     <row r="936">
-      <c r="B936" s="14"/>
+      <c r="B936" s="15"/>
     </row>
     <row r="937">
-      <c r="B937" s="14"/>
+      <c r="B937" s="15"/>
     </row>
     <row r="938">
-      <c r="B938" s="14"/>
+      <c r="B938" s="15"/>
     </row>
     <row r="939">
-      <c r="B939" s="14"/>
+      <c r="B939" s="15"/>
     </row>
     <row r="940">
-      <c r="B940" s="14"/>
+      <c r="B940" s="15"/>
     </row>
     <row r="941">
-      <c r="B941" s="14"/>
+      <c r="B941" s="15"/>
     </row>
     <row r="942">
-      <c r="B942" s="14"/>
+      <c r="B942" s="15"/>
     </row>
     <row r="943">
-      <c r="B943" s="14"/>
+      <c r="B943" s="15"/>
     </row>
     <row r="944">
-      <c r="B944" s="14"/>
+      <c r="B944" s="15"/>
     </row>
     <row r="945">
-      <c r="B945" s="14"/>
+      <c r="B945" s="15"/>
     </row>
     <row r="946">
-      <c r="B946" s="14"/>
+      <c r="B946" s="15"/>
     </row>
     <row r="947">
-      <c r="B947" s="14"/>
+      <c r="B947" s="15"/>
     </row>
     <row r="948">
-      <c r="B948" s="14"/>
+      <c r="B948" s="15"/>
     </row>
     <row r="949">
-      <c r="B949" s="14"/>
+      <c r="B949" s="15"/>
     </row>
     <row r="950">
-      <c r="B950" s="14"/>
+      <c r="B950" s="15"/>
     </row>
     <row r="951">
-      <c r="B951" s="14"/>
+      <c r="B951" s="15"/>
     </row>
     <row r="952">
-      <c r="B952" s="14"/>
+      <c r="B952" s="15"/>
     </row>
     <row r="953">
-      <c r="B953" s="14"/>
+      <c r="B953" s="15"/>
     </row>
     <row r="954">
-      <c r="B954" s="14"/>
+      <c r="B954" s="15"/>
     </row>
     <row r="955">
-      <c r="B955" s="14"/>
+      <c r="B955" s="15"/>
     </row>
     <row r="956">
-      <c r="B956" s="14"/>
+      <c r="B956" s="15"/>
     </row>
     <row r="957">
-      <c r="B957" s="14"/>
+      <c r="B957" s="15"/>
     </row>
     <row r="958">
-      <c r="B958" s="14"/>
+      <c r="B958" s="15"/>
     </row>
     <row r="959">
-      <c r="B959" s="14"/>
+      <c r="B959" s="15"/>
     </row>
     <row r="960">
-      <c r="B960" s="14"/>
+      <c r="B960" s="15"/>
     </row>
     <row r="961">
-      <c r="B961" s="14"/>
+      <c r="B961" s="15"/>
     </row>
     <row r="962">
-      <c r="B962" s="14"/>
+      <c r="B962" s="15"/>
     </row>
     <row r="963">
-      <c r="B963" s="14"/>
+      <c r="B963" s="15"/>
     </row>
     <row r="964">
-      <c r="B964" s="14"/>
+      <c r="B964" s="15"/>
     </row>
     <row r="965">
-      <c r="B965" s="14"/>
+      <c r="B965" s="15"/>
     </row>
     <row r="966">
-      <c r="B966" s="14"/>
+      <c r="B966" s="15"/>
     </row>
     <row r="967">
-      <c r="B967" s="14"/>
+      <c r="B967" s="15"/>
     </row>
     <row r="968">
-      <c r="B968" s="14"/>
+      <c r="B968" s="15"/>
     </row>
     <row r="969">
-      <c r="B969" s="14"/>
+      <c r="B969" s="15"/>
     </row>
     <row r="970">
-      <c r="B970" s="14"/>
+      <c r="B970" s="15"/>
     </row>
     <row r="971">
-      <c r="B971" s="14"/>
+      <c r="B971" s="15"/>
     </row>
     <row r="972">
-      <c r="B972" s="14"/>
+      <c r="B972" s="15"/>
     </row>
     <row r="973">
-      <c r="B973" s="14"/>
+      <c r="B973" s="15"/>
     </row>
     <row r="974">
-      <c r="B974" s="14"/>
+      <c r="B974" s="15"/>
     </row>
     <row r="975">
-      <c r="B975" s="14"/>
+      <c r="B975" s="15"/>
     </row>
     <row r="976">
-      <c r="B976" s="14"/>
+      <c r="B976" s="15"/>
     </row>
     <row r="977">
-      <c r="B977" s="14"/>
+      <c r="B977" s="15"/>
     </row>
     <row r="978">
-      <c r="B978" s="14"/>
+      <c r="B978" s="15"/>
     </row>
     <row r="979">
-      <c r="B979" s="14"/>
+      <c r="B979" s="15"/>
     </row>
     <row r="980">
-      <c r="B980" s="14"/>
+      <c r="B980" s="15"/>
     </row>
     <row r="981">
-      <c r="B981" s="14"/>
+      <c r="B981" s="15"/>
     </row>
     <row r="982">
-      <c r="B982" s="14"/>
+      <c r="B982" s="15"/>
     </row>
     <row r="983">
-      <c r="B983" s="14"/>
+      <c r="B983" s="15"/>
     </row>
     <row r="984">
-      <c r="B984" s="14"/>
+      <c r="B984" s="15"/>
     </row>
     <row r="985">
-      <c r="B985" s="14"/>
+      <c r="B985" s="15"/>
     </row>
     <row r="986">
-      <c r="B986" s="14"/>
+      <c r="B986" s="15"/>
     </row>
     <row r="987">
-      <c r="B987" s="14"/>
+      <c r="B987" s="15"/>
     </row>
     <row r="988">
-      <c r="B988" s="14"/>
+      <c r="B988" s="15"/>
     </row>
     <row r="989">
-      <c r="B989" s="14"/>
+      <c r="B989" s="15"/>
     </row>
     <row r="990">
-      <c r="B990" s="14"/>
+      <c r="B990" s="15"/>
     </row>
     <row r="991">
-      <c r="B991" s="14"/>
+      <c r="B991" s="15"/>
     </row>
     <row r="992">
-      <c r="B992" s="14"/>
+      <c r="B992" s="15"/>
     </row>
     <row r="993">
-      <c r="B993" s="14"/>
+      <c r="B993" s="15"/>
     </row>
     <row r="994">
-      <c r="B994" s="14"/>
+      <c r="B994" s="15"/>
     </row>
     <row r="995">
-      <c r="B995" s="14"/>
+      <c r="B995" s="15"/>
     </row>
     <row r="996">
-      <c r="B996" s="14"/>
+      <c r="B996" s="15"/>
     </row>
     <row r="997">
-      <c r="B997" s="14"/>
+      <c r="B997" s="15"/>
     </row>
     <row r="998">
-      <c r="B998" s="14"/>
+      <c r="B998" s="15"/>
     </row>
     <row r="999">
-      <c r="B999" s="14"/>
+      <c r="B999" s="15"/>
     </row>
     <row r="1000">
-      <c r="B1000" s="14"/>
+      <c r="B1000" s="15"/>
     </row>
     <row r="1001">
-      <c r="B1001" s="14"/>
+      <c r="B1001" s="15"/>
     </row>
     <row r="1002">
-      <c r="B1002" s="14"/>
+      <c r="B1002" s="15"/>
     </row>
     <row r="1003">
-      <c r="B1003" s="14"/>
+      <c r="B1003" s="15"/>
     </row>
     <row r="1004">
-      <c r="B1004" s="14"/>
+      <c r="B1004" s="15"/>
     </row>
     <row r="1005">
-      <c r="B1005" s="14"/>
+      <c r="B1005" s="15"/>
     </row>
     <row r="1006">
-      <c r="B1006" s="14"/>
+      <c r="B1006" s="15"/>
     </row>
     <row r="1007">
-      <c r="B1007" s="14"/>
+      <c r="B1007" s="15"/>
     </row>
     <row r="1008">
-      <c r="B1008" s="14"/>
+      <c r="B1008" s="15"/>
     </row>
     <row r="1009">
-      <c r="B1009" s="14"/>
+      <c r="B1009" s="15"/>
     </row>
     <row r="1010">
-      <c r="B1010" s="14"/>
+      <c r="B1010" s="15"/>
     </row>
     <row r="1011">
-      <c r="B1011" s="14"/>
+      <c r="B1011" s="15"/>
     </row>
     <row r="1012">
-      <c r="B1012" s="14"/>
+      <c r="B1012" s="15"/>
     </row>
     <row r="1013">
-      <c r="B1013" s="14"/>
+      <c r="B1013" s="15"/>
     </row>
     <row r="1014">
-      <c r="B1014" s="14"/>
+      <c r="B1014" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B14"/>
-    <hyperlink r:id="rId5" ref="B15"/>
-    <hyperlink r:id="rId6" ref="B16"/>
-    <hyperlink r:id="rId7" ref="B17"/>
-    <hyperlink r:id="rId8" ref="B19"/>
-    <hyperlink r:id="rId9" ref="B20"/>
-    <hyperlink r:id="rId10" ref="B21"/>
-    <hyperlink r:id="rId11" ref="B22"/>
-    <hyperlink r:id="rId12" ref="B23"/>
-    <hyperlink r:id="rId13" ref="B25"/>
-    <hyperlink r:id="rId14" ref="B28"/>
-    <hyperlink r:id="rId15" ref="B29"/>
-    <hyperlink r:id="rId16" ref="B31"/>
-    <hyperlink r:id="rId17" ref="B32"/>
-    <hyperlink r:id="rId18" ref="B33"/>
-    <hyperlink r:id="rId19" ref="B34"/>
-    <hyperlink r:id="rId20" ref="B35"/>
-    <hyperlink r:id="rId21" ref="B36"/>
-    <hyperlink r:id="rId22" ref="B37"/>
-    <hyperlink r:id="rId23" ref="B38"/>
-    <hyperlink r:id="rId24" ref="B39"/>
-    <hyperlink r:id="rId25" ref="B40"/>
+    <hyperlink r:id="rId1" ref="B5"/>
+    <hyperlink r:id="rId2" ref="B6"/>
+    <hyperlink r:id="rId3" ref="B7"/>
+    <hyperlink r:id="rId4" ref="B8"/>
+    <hyperlink r:id="rId5" ref="B9"/>
+    <hyperlink r:id="rId6" ref="B10"/>
+    <hyperlink r:id="rId7" ref="B11"/>
+    <hyperlink r:id="rId8" ref="B12"/>
+    <hyperlink r:id="rId9" ref="B13"/>
+    <hyperlink r:id="rId10" ref="B18"/>
+    <hyperlink r:id="rId11" ref="B24"/>
+    <hyperlink r:id="rId12" ref="B26"/>
+    <hyperlink r:id="rId13" ref="B27"/>
+    <hyperlink r:id="rId14" ref="B29"/>
+    <hyperlink r:id="rId15" ref="B30"/>
   </hyperlinks>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>